<commit_message>
feat(buck design): :sparkles: Completed first block
- Need to check if Vin is limited by Buck input impedance
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/skim281_uoa_auckland_ac_nz/Documents/Teaching/Electeng 734/2024/EE734 Design Report Student Package 2024/Buck/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{9E39B521-AEE0-4171-AA04-20CBDCC6E229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F1A72EC-1E1C-4EE8-98B7-718991223F9A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC68ADF-1814-4D91-A200-C26CCE8B3D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1811,26 +1811,28 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -1852,7 +1854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
@@ -1863,7 +1865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
@@ -1885,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1907,7 +1909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -1918,16 +1920,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
@@ -1950,7 +1952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="68" t="s">
         <v>229</v>
       </c>
@@ -1973,99 +1975,129 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="10">
+        <v>17.547000000000001</v>
+      </c>
       <c r="C19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10">
+        <v>17.55</v>
+      </c>
       <c r="E19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="10">
+        <v>9.41</v>
+      </c>
       <c r="G19" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="10"/>
+      <c r="B20">
+        <v>2.96</v>
+      </c>
       <c r="C20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10">
+        <v>2.1</v>
+      </c>
       <c r="E20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="10">
+        <v>1.325</v>
+      </c>
       <c r="G20" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B21" s="10">
+        <v>1.3</v>
+      </c>
       <c r="C21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10">
+        <v>1.3</v>
+      </c>
       <c r="E21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="10">
+        <v>0.77400000000000002</v>
+      </c>
       <c r="G21" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="10">
+        <v>43.88</v>
+      </c>
       <c r="C22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10">
+        <v>62.07</v>
+      </c>
       <c r="E22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="10">
+        <v>71.849999999999994</v>
+      </c>
       <c r="G22" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="19">
+        <v>5.9240000000000004</v>
+      </c>
       <c r="C23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="19">
+        <v>8.3800000000000008</v>
+      </c>
       <c r="E23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="19">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="G23" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>5</v>
       </c>
@@ -2076,7 +2108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
@@ -2088,7 +2120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
@@ -2100,7 +2132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>31</v>
       </c>
@@ -2109,7 +2141,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>29</v>
       </c>
@@ -2118,23 +2150,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
@@ -2156,14 +2188,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>5</v>
       </c>
@@ -2186,7 +2218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A44" s="68" t="s">
         <v>229</v>
       </c>
@@ -2209,7 +2241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
         <v>36</v>
       </c>
@@ -2226,7 +2258,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
         <v>37</v>
       </c>
@@ -2243,7 +2275,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
         <v>39</v>
       </c>
@@ -2260,7 +2292,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
         <v>158</v>
       </c>
@@ -2277,7 +2309,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
         <v>38</v>
       </c>
@@ -2294,14 +2326,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
     </row>
   </sheetData>
@@ -2321,28 +2353,28 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.625" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2353,7 +2385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>49</v>
       </c>
@@ -2365,7 +2397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>48</v>
       </c>
@@ -2374,7 +2406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
         <v>50</v>
       </c>
@@ -2383,7 +2415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>60</v>
       </c>
@@ -2406,7 +2438,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>62</v>
       </c>
@@ -2417,14 +2449,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
@@ -2435,7 +2467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>52</v>
       </c>
@@ -2444,7 +2476,7 @@
       </c>
       <c r="C17" s="28"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
         <v>53</v>
       </c>
@@ -2453,7 +2485,7 @@
       </c>
       <c r="C18" s="38"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>54</v>
       </c>
@@ -2464,7 +2496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>58</v>
       </c>
@@ -2475,7 +2507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
         <v>57</v>
       </c>
@@ -2486,7 +2518,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>55</v>
       </c>
@@ -2497,7 +2529,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="46" t="s">
         <v>56</v>
       </c>
@@ -2508,7 +2540,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
         <v>66</v>
       </c>
@@ -2520,7 +2552,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
         <v>67</v>
       </c>
@@ -2532,7 +2564,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="47" t="s">
         <v>65</v>
       </c>
@@ -2541,23 +2573,23 @@
       </c>
       <c r="C26" s="42"/>
     </row>
-    <row r="27" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>5</v>
       </c>
@@ -2568,7 +2600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" s="45" t="s">
         <v>230</v>
       </c>
@@ -2579,7 +2611,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="47" t="s">
         <v>221</v>
       </c>
@@ -2591,17 +2623,17 @@
       </c>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -2612,7 +2644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A39" s="45" t="s">
         <v>73</v>
       </c>
@@ -2621,7 +2653,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
         <v>77</v>
       </c>
@@ -2630,7 +2662,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="46" t="s">
         <v>81</v>
       </c>
@@ -2639,7 +2671,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="46" t="s">
         <v>80</v>
       </c>
@@ -2648,7 +2680,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="46" t="s">
         <v>83</v>
       </c>
@@ -2657,7 +2689,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="46" t="s">
         <v>86</v>
       </c>
@@ -2667,7 +2699,7 @@
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="47" t="s">
         <v>88</v>
       </c>
@@ -2676,14 +2708,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>5</v>
       </c>
@@ -2706,7 +2738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A51" s="69" t="s">
         <v>229</v>
       </c>
@@ -2729,7 +2761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="46" t="s">
         <v>39</v>
       </c>
@@ -2746,7 +2778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="46" t="s">
         <v>36</v>
       </c>
@@ -2763,7 +2795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="46" t="s">
         <v>92</v>
       </c>
@@ -2780,7 +2812,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="46" t="s">
         <v>93</v>
       </c>
@@ -2797,7 +2829,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="46" t="s">
         <v>94</v>
       </c>
@@ -2814,7 +2846,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="47" t="s">
         <v>95</v>
       </c>
@@ -2831,7 +2863,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2850,24 +2882,24 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2878,7 +2910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>102</v>
       </c>
@@ -2890,7 +2922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>104</v>
       </c>
@@ -2899,7 +2931,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
         <v>205</v>
       </c>
@@ -2908,7 +2940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>103</v>
       </c>
@@ -2920,7 +2952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>106</v>
       </c>
@@ -2931,14 +2963,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
@@ -2949,7 +2981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
         <v>224</v>
       </c>
@@ -2958,7 +2990,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="47" t="s">
         <v>108</v>
       </c>
@@ -2967,14 +2999,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>5</v>
       </c>
@@ -2985,7 +3017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
         <v>112</v>
       </c>
@@ -2994,7 +3026,7 @@
       </c>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
         <v>111</v>
       </c>
@@ -3003,7 +3035,7 @@
       </c>
       <c r="C24" s="38"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
         <v>115</v>
       </c>
@@ -3012,7 +3044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="46" t="s">
         <v>225</v>
       </c>
@@ -3021,7 +3053,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
         <v>117</v>
       </c>
@@ -3030,7 +3062,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="47" t="s">
         <v>119</v>
       </c>
@@ -3039,14 +3071,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>5</v>
       </c>
@@ -3069,7 +3101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="69" t="s">
         <v>229</v>
       </c>
@@ -3092,7 +3124,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="46" t="s">
         <v>38</v>
       </c>
@@ -3109,7 +3141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="47" t="s">
         <v>121</v>
       </c>
@@ -3126,7 +3158,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3145,24 +3177,24 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -3173,7 +3205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>123</v>
       </c>
@@ -3185,7 +3217,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>159</v>
       </c>
@@ -3194,7 +3226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
         <v>125</v>
       </c>
@@ -3203,7 +3235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>124</v>
       </c>
@@ -3215,7 +3247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="47" t="s">
         <v>126</v>
       </c>
@@ -3226,14 +3258,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
@@ -3244,21 +3276,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="37"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>129</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="38"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
         <v>130</v>
       </c>
@@ -3267,7 +3299,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>131</v>
       </c>
@@ -3276,7 +3308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>132</v>
       </c>
@@ -3285,7 +3317,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
         <v>133</v>
       </c>
@@ -3294,7 +3326,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>135</v>
       </c>
@@ -3303,7 +3335,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="46" t="s">
         <v>138</v>
       </c>
@@ -3312,7 +3344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="46" t="s">
         <v>137</v>
       </c>
@@ -3321,7 +3353,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="47" t="s">
         <v>165</v>
       </c>
@@ -3330,14 +3362,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>5</v>
       </c>
@@ -3348,7 +3380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A30" s="45" t="s">
         <v>150</v>
       </c>
@@ -3359,7 +3391,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="46" t="s">
         <v>151</v>
       </c>
@@ -3370,7 +3402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="47" t="s">
         <v>147</v>
       </c>
@@ -3379,16 +3411,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -3411,7 +3443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A38" s="69" t="s">
         <v>229</v>
       </c>
@@ -3434,7 +3466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="46" t="s">
         <v>140</v>
       </c>
@@ -3451,7 +3483,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
         <v>157</v>
       </c>
@@ -3468,7 +3500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="46" t="s">
         <v>36</v>
       </c>
@@ -3485,7 +3517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="46" t="s">
         <v>160</v>
       </c>
@@ -3502,7 +3534,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="46" t="s">
         <v>161</v>
       </c>
@@ -3519,7 +3551,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="46" t="s">
         <v>143</v>
       </c>
@@ -3536,7 +3568,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="46" t="s">
         <v>144</v>
       </c>
@@ -3553,7 +3585,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="46" t="s">
         <v>152</v>
       </c>
@@ -3570,7 +3602,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="46" t="s">
         <v>153</v>
       </c>
@@ -3587,7 +3619,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="46" t="s">
         <v>156</v>
       </c>
@@ -3604,7 +3636,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="46" t="s">
         <v>162</v>
       </c>
@@ -3621,7 +3653,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="47" t="s">
         <v>95</v>
       </c>
@@ -3638,14 +3670,14 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
@@ -3656,7 +3688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="52" t="s">
         <v>166</v>
       </c>
@@ -3665,7 +3697,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3684,24 +3716,24 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -3712,7 +3744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>168</v>
       </c>
@@ -3724,7 +3756,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>169</v>
       </c>
@@ -3733,7 +3765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
         <v>124</v>
       </c>
@@ -3745,7 +3777,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="47" t="s">
         <v>126</v>
       </c>
@@ -3756,14 +3788,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
@@ -3774,21 +3806,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="37"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
         <v>129</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="38"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>171</v>
       </c>
@@ -3797,7 +3829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
         <v>172</v>
       </c>
@@ -3806,7 +3838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>173</v>
       </c>
@@ -3815,7 +3847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="47" t="s">
         <v>174</v>
       </c>
@@ -3824,14 +3856,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
@@ -3854,7 +3886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="69" t="s">
         <v>229</v>
       </c>
@@ -3877,7 +3909,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
         <v>140</v>
       </c>
@@ -3894,7 +3926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="46" t="s">
         <v>9</v>
       </c>
@@ -3911,7 +3943,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="46" t="s">
         <v>175</v>
       </c>
@@ -3928,7 +3960,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="46" t="s">
         <v>162</v>
       </c>
@@ -3945,7 +3977,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="46" t="s">
         <v>177</v>
       </c>
@@ -3962,7 +3994,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="47" t="s">
         <v>95</v>
       </c>
@@ -3979,14 +4011,14 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -3997,7 +4029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="52" t="s">
         <v>166</v>
       </c>
@@ -4006,7 +4038,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4021,29 +4053,29 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="73" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="3" width="11.875" customWidth="1"/>
-    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" customWidth="1"/>
+    <col min="2" max="3" width="11.8984375" customWidth="1"/>
+    <col min="4" max="4" width="22.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -4054,7 +4086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="45" t="s">
         <v>222</v>
       </c>
@@ -4066,7 +4098,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="46" t="s">
         <v>206</v>
       </c>
@@ -4078,7 +4110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="46" t="s">
         <v>183</v>
       </c>
@@ -4090,7 +4122,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="46" t="s">
         <v>117</v>
       </c>
@@ -4102,7 +4134,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>124</v>
       </c>
@@ -4114,7 +4146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="47" t="s">
         <v>190</v>
       </c>
@@ -4125,14 +4157,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
@@ -4143,7 +4175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>185</v>
       </c>
@@ -4154,7 +4186,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
         <v>186</v>
       </c>
@@ -4163,7 +4195,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="47" t="s">
         <v>189</v>
       </c>
@@ -4172,14 +4204,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>5</v>
       </c>
@@ -4190,7 +4222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
         <v>192</v>
       </c>
@@ -4199,7 +4231,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="53" t="s">
         <v>226</v>
       </c>
@@ -4210,7 +4242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="54" t="s">
         <v>227</v>
       </c>
@@ -4219,14 +4251,14 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
@@ -4237,7 +4269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
         <v>209</v>
       </c>
@@ -4246,7 +4278,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="46" t="s">
         <v>208</v>
       </c>
@@ -4255,7 +4287,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="46" t="s">
         <v>199</v>
       </c>
@@ -4265,7 +4297,7 @@
       </c>
       <c r="D35" s="70"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="46" t="s">
         <v>210</v>
       </c>
@@ -4276,7 +4308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="46" t="s">
         <v>207</v>
       </c>
@@ -4285,7 +4317,7 @@
       </c>
       <c r="C37" s="38"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="46" t="s">
         <v>215</v>
       </c>
@@ -4295,7 +4327,7 @@
       </c>
       <c r="D38" s="70"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="46" t="s">
         <v>217</v>
       </c>
@@ -4304,7 +4336,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
         <v>211</v>
       </c>
@@ -4315,7 +4347,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="46" t="s">
         <v>212</v>
       </c>
@@ -4324,7 +4356,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="46" t="s">
         <v>213</v>
       </c>
@@ -4333,7 +4365,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="47" t="s">
         <v>223</v>
       </c>
@@ -4342,8 +4374,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
feat(buck design): :sparkles: Saving work
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC68ADF-1814-4D91-A200-C26CCE8B3D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90E84F4-CE02-4306-8744-D4DA9D45C3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="0" windowWidth="21600" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1811,8 +1811,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2038,7 +2038,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="10">
-        <v>0.77400000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>20</v>
@@ -2136,7 +2136,9 @@
       <c r="A31" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="10">
+        <v>71.849999999999994</v>
+      </c>
       <c r="C31" s="24" t="s">
         <v>21</v>
       </c>
@@ -2145,7 +2147,9 @@
       <c r="A32" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="19">
+        <v>10.27</v>
+      </c>
       <c r="C32" s="21" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
feat(buck-design): :sparkles: Finished operating conditions sheet
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90E84F4-CE02-4306-8744-D4DA9D45C3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0401DCE-8E0C-401E-B02E-6D066C940717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="0" windowWidth="21600" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="15624" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1811,8 +1811,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2249,15 +2249,21 @@
       <c r="A45" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="10"/>
+      <c r="B45" s="10">
+        <v>1.33</v>
+      </c>
       <c r="C45" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="10"/>
+      <c r="D45" s="10">
+        <v>1.27</v>
+      </c>
       <c r="E45" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F45" s="10"/>
+      <c r="F45" s="10">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="G45" s="17" t="s">
         <v>41</v>
       </c>
@@ -2266,15 +2272,21 @@
       <c r="A46" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="10"/>
+      <c r="B46" s="10">
+        <v>3.63</v>
+      </c>
       <c r="C46" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D46" s="10"/>
+      <c r="D46" s="10">
+        <v>2.74</v>
+      </c>
       <c r="E46" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F46" s="10"/>
+      <c r="F46" s="10">
+        <v>1.88</v>
+      </c>
       <c r="G46" s="17" t="s">
         <v>42</v>
       </c>
@@ -2283,15 +2295,21 @@
       <c r="A47" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="10"/>
+      <c r="B47" s="10">
+        <v>2.98</v>
+      </c>
       <c r="C47" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="10">
+        <v>2.13</v>
+      </c>
       <c r="E47" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F47" s="10"/>
+      <c r="F47" s="10">
+        <v>1.367</v>
+      </c>
       <c r="G47" s="17" t="s">
         <v>43</v>
       </c>
@@ -2300,15 +2318,21 @@
       <c r="A48" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="10"/>
+      <c r="B48" s="10">
+        <v>1.98</v>
+      </c>
       <c r="C48" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="10"/>
+      <c r="D48" s="10">
+        <v>1.68</v>
+      </c>
       <c r="E48" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F48" s="10"/>
+      <c r="F48" s="10">
+        <v>1.1599999999999999</v>
+      </c>
       <c r="G48" s="17" t="s">
         <v>44</v>
       </c>
@@ -2317,15 +2341,21 @@
       <c r="A49" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="19"/>
+      <c r="B49" s="19">
+        <v>0.38</v>
+      </c>
       <c r="C49" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="19"/>
+      <c r="D49" s="19">
+        <v>0.37</v>
+      </c>
       <c r="E49" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="19"/>
+      <c r="F49" s="19">
+        <v>0.31</v>
+      </c>
       <c r="G49" s="21" t="s">
         <v>45</v>
       </c>
@@ -4108,7 +4138,7 @@
       </c>
       <c r="B7" s="55">
         <f>'Operating Conditions'!B46</f>
-        <v>0</v>
+        <v>3.63</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
feat(buck-design): :sparkles: Added equations for buck
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0401DCE-8E0C-401E-B02E-6D066C940717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1861CAA8-AC6C-4C2E-86A3-1BC654C40158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="15624" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -1811,28 +1811,28 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A25" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="7" width="11.8984375" customWidth="1"/>
+    <col min="2" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -1920,16 +1920,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="68" t="s">
         <v>229</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>8</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>9</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
@@ -2090,14 +2090,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>5</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>31</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>29</v>
       </c>
@@ -2154,23 +2154,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
@@ -2192,14 +2192,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>5</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A44" s="68" t="s">
         <v>229</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>36</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>37</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>39</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>158</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>38</v>
       </c>
@@ -2360,14 +2360,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
     </row>
   </sheetData>
@@ -2387,28 +2387,28 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView topLeftCell="A37" zoomScale="77" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.59765625" customWidth="1"/>
-    <col min="2" max="7" width="11.8984375" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="2" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
         <v>49</v>
       </c>
@@ -2431,25 +2431,29 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="32">
+        <v>3.63</v>
+      </c>
       <c r="C7" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="32">
+        <v>2.98</v>
+      </c>
       <c r="C8" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>25</v>
       </c>
@@ -2461,7 +2465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
         <v>60</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>62</v>
       </c>
@@ -2483,14 +2487,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
@@ -2501,7 +2505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>52</v>
       </c>
@@ -2510,7 +2514,7 @@
       </c>
       <c r="C17" s="28"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>53</v>
       </c>
@@ -2519,7 +2523,7 @@
       </c>
       <c r="C18" s="38"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>54</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
         <v>58</v>
       </c>
@@ -2541,7 +2545,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
         <v>57</v>
       </c>
@@ -2552,7 +2556,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>55</v>
       </c>
@@ -2563,7 +2567,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
         <v>56</v>
       </c>
@@ -2574,7 +2578,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>66</v>
       </c>
@@ -2586,7 +2590,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
         <v>67</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="47" t="s">
         <v>65</v>
       </c>
@@ -2607,23 +2611,23 @@
       </c>
       <c r="C26" s="42"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>5</v>
       </c>
@@ -2634,7 +2638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
         <v>230</v>
       </c>
@@ -2645,7 +2649,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="47" t="s">
         <v>221</v>
       </c>
@@ -2657,17 +2661,17 @@
       </c>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -2678,7 +2682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
         <v>73</v>
       </c>
@@ -2687,7 +2691,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
         <v>77</v>
       </c>
@@ -2696,7 +2700,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>81</v>
       </c>
@@ -2705,7 +2709,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
         <v>80</v>
       </c>
@@ -2714,7 +2718,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
         <v>83</v>
       </c>
@@ -2723,7 +2727,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
         <v>86</v>
       </c>
@@ -2733,7 +2737,7 @@
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="47" t="s">
         <v>88</v>
       </c>
@@ -2742,14 +2746,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>5</v>
       </c>
@@ -2772,7 +2776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="69" t="s">
         <v>229</v>
       </c>
@@ -2795,7 +2799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
         <v>39</v>
       </c>
@@ -2812,7 +2816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
         <v>36</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
         <v>92</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="46" t="s">
         <v>93</v>
       </c>
@@ -2863,7 +2867,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
         <v>94</v>
       </c>
@@ -2880,7 +2884,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="47" t="s">
         <v>95</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2912,28 +2916,28 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" customWidth="1"/>
-    <col min="2" max="7" width="11.8984375" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="2" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
         <v>102</v>
       </c>
@@ -2956,7 +2960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>104</v>
       </c>
@@ -2965,7 +2969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>205</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>103</v>
       </c>
@@ -2986,7 +2990,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>106</v>
       </c>
@@ -2997,14 +3001,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
@@ -3015,7 +3019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>224</v>
       </c>
@@ -3024,7 +3028,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47" t="s">
         <v>108</v>
       </c>
@@ -3033,14 +3037,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>5</v>
       </c>
@@ -3051,7 +3055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
         <v>112</v>
       </c>
@@ -3060,7 +3064,7 @@
       </c>
       <c r="C23" s="37"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>111</v>
       </c>
@@ -3069,7 +3073,7 @@
       </c>
       <c r="C24" s="38"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
         <v>115</v>
       </c>
@@ -3078,7 +3082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
         <v>225</v>
       </c>
@@ -3087,7 +3091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
         <v>117</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47" t="s">
         <v>119</v>
       </c>
@@ -3105,14 +3109,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>5</v>
       </c>
@@ -3135,7 +3139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" s="69" t="s">
         <v>229</v>
       </c>
@@ -3158,7 +3162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
         <v>38</v>
       </c>
@@ -3175,7 +3179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="47" t="s">
         <v>121</v>
       </c>
@@ -3192,7 +3196,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3207,28 +3211,28 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.8984375" customWidth="1"/>
-    <col min="2" max="7" width="11.8984375" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -3239,7 +3243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
         <v>123</v>
       </c>
@@ -3251,7 +3255,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>159</v>
       </c>
@@ -3260,7 +3264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>125</v>
       </c>
@@ -3269,7 +3273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>124</v>
       </c>
@@ -3281,7 +3285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>126</v>
       </c>
@@ -3292,14 +3296,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
@@ -3310,21 +3314,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="37"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
         <v>129</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="38"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>130</v>
       </c>
@@ -3333,7 +3337,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>131</v>
       </c>
@@ -3342,7 +3346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
         <v>132</v>
       </c>
@@ -3351,7 +3355,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
         <v>133</v>
       </c>
@@ -3360,7 +3364,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>135</v>
       </c>
@@ -3369,7 +3373,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
         <v>138</v>
       </c>
@@ -3378,7 +3382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>137</v>
       </c>
@@ -3387,7 +3391,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="47" t="s">
         <v>165</v>
       </c>
@@ -3396,14 +3400,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>5</v>
       </c>
@@ -3414,7 +3418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
         <v>150</v>
       </c>
@@ -3425,7 +3429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
         <v>151</v>
       </c>
@@ -3436,7 +3440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47" t="s">
         <v>147</v>
       </c>
@@ -3445,16 +3449,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -3477,7 +3481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="69" t="s">
         <v>229</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
         <v>140</v>
       </c>
@@ -3517,7 +3521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
         <v>157</v>
       </c>
@@ -3534,7 +3538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>36</v>
       </c>
@@ -3551,7 +3555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
         <v>160</v>
       </c>
@@ -3568,7 +3572,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
         <v>161</v>
       </c>
@@ -3585,7 +3589,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
         <v>143</v>
       </c>
@@ -3602,7 +3606,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
         <v>144</v>
       </c>
@@ -3619,7 +3623,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
         <v>152</v>
       </c>
@@ -3636,7 +3640,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
         <v>153</v>
       </c>
@@ -3653,7 +3657,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
         <v>156</v>
       </c>
@@ -3670,7 +3674,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
         <v>162</v>
       </c>
@@ -3687,7 +3691,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="47" t="s">
         <v>95</v>
       </c>
@@ -3704,14 +3708,14 @@
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
@@ -3722,7 +3726,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="52" t="s">
         <v>166</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3746,28 +3750,28 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.09765625" customWidth="1"/>
-    <col min="2" max="7" width="11.8984375" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="7" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -3778,7 +3782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
         <v>168</v>
       </c>
@@ -3790,7 +3794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>169</v>
       </c>
@@ -3799,7 +3803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>124</v>
       </c>
@@ -3811,7 +3815,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>126</v>
       </c>
@@ -3822,14 +3826,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
@@ -3840,21 +3844,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="37"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
         <v>129</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="38"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
         <v>171</v>
       </c>
@@ -3863,7 +3867,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>172</v>
       </c>
@@ -3872,7 +3876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>173</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47" t="s">
         <v>174</v>
       </c>
@@ -3890,14 +3894,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
         <v>229</v>
       </c>
@@ -3943,7 +3947,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
         <v>140</v>
       </c>
@@ -3960,7 +3964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
         <v>9</v>
       </c>
@@ -3977,7 +3981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
         <v>175</v>
       </c>
@@ -3994,7 +3998,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
         <v>162</v>
       </c>
@@ -4011,7 +4015,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
         <v>177</v>
       </c>
@@ -4028,7 +4032,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47" t="s">
         <v>95</v>
       </c>
@@ -4045,14 +4049,14 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -4063,7 +4067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="52" t="s">
         <v>166</v>
       </c>
@@ -4072,7 +4076,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4091,25 +4095,25 @@
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" customWidth="1"/>
-    <col min="2" max="3" width="11.8984375" customWidth="1"/>
-    <col min="4" max="4" width="22.69921875" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -4120,7 +4124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
         <v>222</v>
       </c>
@@ -4132,7 +4136,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>206</v>
       </c>
@@ -4144,7 +4148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>183</v>
       </c>
@@ -4156,7 +4160,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>117</v>
       </c>
@@ -4168,7 +4172,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
         <v>124</v>
       </c>
@@ -4180,7 +4184,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>190</v>
       </c>
@@ -4191,14 +4195,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
@@ -4209,7 +4213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>185</v>
       </c>
@@ -4220,7 +4224,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>186</v>
       </c>
@@ -4229,7 +4233,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47" t="s">
         <v>189</v>
       </c>
@@ -4238,14 +4242,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>5</v>
       </c>
@@ -4256,7 +4260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
         <v>192</v>
       </c>
@@ -4265,7 +4269,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>226</v>
       </c>
@@ -4276,7 +4280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="54" t="s">
         <v>227</v>
       </c>
@@ -4285,14 +4289,14 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
@@ -4303,7 +4307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="45" t="s">
         <v>209</v>
       </c>
@@ -4312,7 +4316,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
         <v>208</v>
       </c>
@@ -4321,7 +4325,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
         <v>199</v>
       </c>
@@ -4331,7 +4335,7 @@
       </c>
       <c r="D35" s="70"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
         <v>210</v>
       </c>
@@ -4342,7 +4346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
         <v>207</v>
       </c>
@@ -4351,7 +4355,7 @@
       </c>
       <c r="C37" s="38"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
         <v>215</v>
       </c>
@@ -4361,7 +4365,7 @@
       </c>
       <c r="D38" s="70"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
         <v>217</v>
       </c>
@@ -4370,7 +4374,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
         <v>211</v>
       </c>
@@ -4381,7 +4385,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>212</v>
       </c>
@@ -4390,7 +4394,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
         <v>213</v>
       </c>
@@ -4399,7 +4403,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="47" t="s">
         <v>223</v>
       </c>
@@ -4408,8 +4412,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
feat(buck-design): :sparkles: Finished inductor design, missing losses
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1861CAA8-AC6C-4C2E-86A3-1BC654C40158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F470FBD-F597-4086-AFE6-E240D3EC11EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="232">
   <si>
     <t>Specifications</t>
   </si>
@@ -738,6 +738,9 @@
   </si>
   <si>
     <t>Selected Air-gap (lg)</t>
+  </si>
+  <si>
+    <t>14 (13.64)</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1267,10 +1270,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -1313,6 +1314,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1847,7 +1863,7 @@
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="58">
         <v>15</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -1858,7 +1874,7 @@
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="61">
+      <c r="B7" s="59">
         <v>1.3</v>
       </c>
       <c r="C7" s="24" t="s">
@@ -1869,7 +1885,7 @@
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="61">
+      <c r="B8" s="59">
         <v>9.6999999999999993</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1880,7 +1896,7 @@
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="61">
+      <c r="B9" s="59">
         <v>10</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -1891,7 +1907,7 @@
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="61">
+      <c r="B10" s="59">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -1902,7 +1918,7 @@
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="61">
+      <c r="B11" s="59">
         <v>90</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -1913,7 +1929,7 @@
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="62">
+      <c r="B12" s="60">
         <v>100</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -1953,22 +1969,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B18" s="60">
+      <c r="B18" s="58">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="58">
         <v>4</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="60">
+      <c r="F18" s="58">
         <v>10</v>
       </c>
       <c r="G18" s="15" t="s">
@@ -2112,7 +2128,7 @@
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="60">
+      <c r="B29" s="58">
         <f>B6</f>
         <v>15</v>
       </c>
@@ -2124,7 +2140,7 @@
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="61">
+      <c r="B30" s="59">
         <f>F18</f>
         <v>10</v>
       </c>
@@ -2185,7 +2201,7 @@
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="71">
+      <c r="B38" s="69">
         <v>25</v>
       </c>
       <c r="C38" s="23" t="s">
@@ -2223,22 +2239,22 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="60">
+      <c r="B44" s="58">
         <v>2</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="60">
+      <c r="D44" s="58">
         <v>4</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="60">
+      <c r="F44" s="58">
         <v>10</v>
       </c>
       <c r="G44" s="15" t="s">
@@ -2387,8 +2403,8 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="77" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2420,10 +2436,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <f>'Operating Conditions'!B38</f>
         <v>25</v>
       </c>
@@ -2432,58 +2448,58 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="32">
         <v>3.63</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="32">
         <v>2.98</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="53">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="53">
         <v>0.25</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="56">
         <v>5</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2506,110 +2522,110 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="61" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="38"/>
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="55">
+      <c r="B19" s="53">
         <v>31</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="37" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="55">
+      <c r="B20" s="53">
         <v>47</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="37" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="55">
+      <c r="B21" s="53">
         <v>1460</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="37" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="55">
+      <c r="B22" s="53">
         <v>28.1</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="37" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="55">
+      <c r="B23" s="53">
         <v>40.200000000000003</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="37" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="65">
+      <c r="B24" s="63">
         <f>1.8*10^-8</f>
         <v>1.8000000000000002E-8</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="65">
+      <c r="B25" s="63">
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="37" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="58">
+      <c r="B26" s="56">
         <v>0.65</v>
       </c>
-      <c r="C26" s="42"/>
+      <c r="C26" s="40"/>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -2639,24 +2655,24 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="56">
+      <c r="B32" s="54">
         <v>0.15</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="B33" s="58">
+      <c r="B33" s="56">
         <v>0.43</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="9"/>
@@ -2683,66 +2699,80 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="37" t="s">
+      <c r="B39" s="70" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="36" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="38" t="s">
+      <c r="B40" s="71">
+        <v>0.22</v>
+      </c>
+      <c r="C40" s="37" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="38" t="s">
+      <c r="B41" s="72">
+        <v>1.4499999999999999E-7</v>
+      </c>
+      <c r="C41" s="37" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="38" t="s">
+      <c r="B42" s="73">
+        <v>9</v>
+      </c>
+      <c r="C42" s="37" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="39"/>
-      <c r="C43" s="38" t="s">
+      <c r="B43" s="72">
+        <v>1.31E-6</v>
+      </c>
+      <c r="C43" s="37" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="38" t="s">
+      <c r="B44" s="71">
+        <v>2.27</v>
+      </c>
+      <c r="C44" s="37" t="s">
         <v>87</v>
       </c>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
+      <c r="A45" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="41"/>
-      <c r="C45" s="42" t="s">
+      <c r="B45" s="74">
+        <v>7.73</v>
+      </c>
+      <c r="C45" s="40" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2777,22 +2807,22 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="67" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="66">
+      <c r="B51" s="64">
         <v>2</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="66">
+      <c r="D51" s="64">
         <v>4</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="66">
+      <c r="F51" s="64">
         <v>10</v>
       </c>
       <c r="G51" s="28" t="s">
@@ -2800,7 +2830,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B52" s="29"/>
@@ -2817,7 +2847,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="44" t="s">
         <v>36</v>
       </c>
       <c r="B53" s="29"/>
@@ -2834,7 +2864,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="46" t="s">
+      <c r="A54" s="44" t="s">
         <v>92</v>
       </c>
       <c r="B54" s="32"/>
@@ -2851,7 +2881,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="44" t="s">
         <v>93</v>
       </c>
       <c r="B55" s="32"/>
@@ -2868,7 +2898,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="44" t="s">
         <v>94</v>
       </c>
       <c r="B56" s="32"/>
@@ -2885,7 +2915,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="45" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="33"/>
@@ -2949,10 +2979,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
@@ -2961,43 +2991,43 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>104</v>
       </c>
       <c r="B7" s="32"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>205</v>
       </c>
       <c r="B8" s="32"/>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="53">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="56">
         <v>1</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3020,20 +3050,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="43"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="28" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="45" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="33"/>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3056,56 +3086,56 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="37"/>
+      <c r="C23" s="36"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="37"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="38" t="s">
+      <c r="B25" s="38"/>
+      <c r="C25" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="40"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="31" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="38" t="s">
+      <c r="B27" s="38"/>
+      <c r="C27" s="37" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="42" t="s">
+      <c r="B28" s="47"/>
+      <c r="C28" s="40" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3140,22 +3170,22 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="67" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="66">
+      <c r="B34" s="64">
         <v>2</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="66">
+      <c r="D34" s="64">
         <v>4</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="66">
+      <c r="F34" s="64">
         <v>10</v>
       </c>
       <c r="G34" s="28" t="s">
@@ -3163,7 +3193,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="44" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="29"/>
@@ -3180,18 +3210,18 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="41"/>
+      <c r="D36" s="39"/>
       <c r="E36" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="41"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="35" t="s">
         <v>141</v>
       </c>
@@ -3244,10 +3274,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -3256,43 +3286,43 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>159</v>
       </c>
       <c r="B7" s="32"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="32"/>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="53">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="56">
         <v>30</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3315,88 +3345,88 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="36"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="38"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="37"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="38" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="38" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="37" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="38" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="37" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="38" t="s">
+      <c r="B22" s="38"/>
+      <c r="C22" s="37" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="38" t="s">
+      <c r="B23" s="38"/>
+      <c r="C23" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="38" t="s">
+      <c r="B24" s="38"/>
+      <c r="C24" s="37" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+      <c r="A25" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="42" t="s">
+      <c r="B25" s="47"/>
+      <c r="C25" s="40" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3419,33 +3449,33 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="56">
+      <c r="B30" s="54">
         <v>15</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="55">
+      <c r="B31" s="53">
         <v>1</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="45" t="s">
         <v>147</v>
       </c>
       <c r="B32" s="33"/>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="40" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3482,22 +3512,22 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="69" t="s">
+      <c r="A38" s="67" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="56">
+      <c r="B38" s="54">
         <v>2</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="66">
+      <c r="D38" s="64">
         <v>4</v>
       </c>
       <c r="E38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="66">
+      <c r="F38" s="64">
         <v>10</v>
       </c>
       <c r="G38" s="28" t="s">
@@ -3505,7 +3535,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="44" t="s">
         <v>140</v>
       </c>
       <c r="B39" s="32"/>
@@ -3522,7 +3552,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="44" t="s">
         <v>157</v>
       </c>
       <c r="B40" s="32"/>
@@ -3539,7 +3569,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="44" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="32"/>
@@ -3556,7 +3586,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="44" t="s">
         <v>160</v>
       </c>
       <c r="B42" s="32"/>
@@ -3573,7 +3603,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="44" t="s">
         <v>161</v>
       </c>
       <c r="B43" s="32"/>
@@ -3590,7 +3620,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="44" t="s">
         <v>143</v>
       </c>
       <c r="B44" s="32"/>
@@ -3607,7 +3637,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B45" s="32"/>
@@ -3624,7 +3654,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="44" t="s">
         <v>152</v>
       </c>
       <c r="B46" s="32"/>
@@ -3641,7 +3671,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="44" t="s">
         <v>153</v>
       </c>
       <c r="B47" s="32"/>
@@ -3658,7 +3688,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="46" t="s">
+      <c r="A48" s="44" t="s">
         <v>156</v>
       </c>
       <c r="B48" s="32"/>
@@ -3675,7 +3705,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="46" t="s">
+      <c r="A49" s="44" t="s">
         <v>162</v>
       </c>
       <c r="B49" s="32"/>
@@ -3692,7 +3722,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="45" t="s">
         <v>95</v>
       </c>
       <c r="B50" s="33"/>
@@ -3727,11 +3757,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="52" t="s">
+      <c r="A56" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="50"/>
-      <c r="C56" s="51" t="s">
+      <c r="B56" s="48"/>
+      <c r="C56" s="49" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3750,8 +3780,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3783,10 +3813,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -3795,34 +3825,34 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>169</v>
       </c>
       <c r="B7" s="32"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="53">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="56">
         <v>30</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3845,52 +3875,52 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="37"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="36"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="37"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="38" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="44" t="s">
         <v>173</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="38" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="42" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="40" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3925,22 +3955,22 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="69" t="s">
+      <c r="A26" s="67" t="s">
         <v>229</v>
       </c>
-      <c r="B26" s="56">
+      <c r="B26" s="54">
         <v>2</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="64">
         <v>4</v>
       </c>
       <c r="E26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="66">
+      <c r="F26" s="64">
         <v>10</v>
       </c>
       <c r="G26" s="28" t="s">
@@ -3948,7 +3978,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="44" t="s">
         <v>140</v>
       </c>
       <c r="B27" s="32"/>
@@ -3965,7 +3995,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="32"/>
@@ -3982,7 +4012,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="44" t="s">
         <v>175</v>
       </c>
       <c r="B29" s="32"/>
@@ -3999,7 +4029,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="44" t="s">
         <v>162</v>
       </c>
       <c r="B30" s="32"/>
@@ -4016,7 +4046,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="44" t="s">
         <v>177</v>
       </c>
       <c r="B31" s="32"/>
@@ -4033,7 +4063,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="45" t="s">
         <v>95</v>
       </c>
       <c r="B32" s="33"/>
@@ -4068,11 +4098,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="51" t="s">
+      <c r="B38" s="48"/>
+      <c r="C38" s="49" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4125,22 +4155,22 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="53">
         <f>'Operating Conditions'!B46</f>
         <v>3.63</v>
       </c>
@@ -4149,10 +4179,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="53">
         <f>Capacitor!B26</f>
         <v>0</v>
       </c>
@@ -4161,37 +4191,37 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="55">
         <f>Capacitor!B27</f>
         <v>0</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="53">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="56">
         <v>5</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4214,31 +4244,31 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="59">
+      <c r="B17" s="57">
         <v>1</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="36" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="38" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="37" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="42" t="s">
+      <c r="B19" s="47"/>
+      <c r="C19" s="40" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4261,31 +4291,31 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="37" t="s">
+      <c r="B25" s="41"/>
+      <c r="C25" s="36" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26" s="53">
         <v>100</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="37" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="52" t="s">
         <v>227</v>
       </c>
       <c r="B27" s="33"/>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="40" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4308,107 +4338,107 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="43" t="s">
         <v>209</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="37" t="s">
+      <c r="B33" s="41"/>
+      <c r="C33" s="36" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="44" t="s">
         <v>208</v>
       </c>
       <c r="B34" s="32"/>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="37" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="44" t="s">
         <v>199</v>
       </c>
       <c r="B35" s="32"/>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="70"/>
+      <c r="D35" s="68"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="55">
+      <c r="B36" s="53">
         <v>10</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="B37" s="55">
+      <c r="B37" s="53">
         <v>1</v>
       </c>
-      <c r="C37" s="38"/>
+      <c r="C37" s="37"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="44" t="s">
         <v>215</v>
       </c>
       <c r="B38" s="32"/>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="D38" s="70"/>
+      <c r="D38" s="68"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="44" t="s">
         <v>217</v>
       </c>
       <c r="B39" s="32"/>
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="37" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="B40" s="55">
+      <c r="B40" s="53">
         <v>22</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="37" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="44" t="s">
         <v>212</v>
       </c>
       <c r="B41" s="32"/>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="37" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="44" t="s">
         <v>213</v>
       </c>
       <c r="B42" s="32"/>
-      <c r="C42" s="38" t="s">
+      <c r="C42" s="37" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="45" t="s">
         <v>223</v>
       </c>
       <c r="B43" s="33"/>
-      <c r="C43" s="42" t="s">
+      <c r="C43" s="40" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(buck-design): :sparkles: Finished capacitor sheet, inductor sheet, halfway done with switch sheet. Equations updated up to capacitor
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F470FBD-F597-4086-AFE6-E240D3EC11EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C986C4-ED45-4A40-8A8E-744E469E1683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="18645" windowHeight="20985" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -44,8 +44,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1135DF8B-2E7F-46E9-B040-718C71944AFB}</author>
+  </authors>
+  <commentList>
+    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{1135DF8B-2E7F-46E9-B040-718C71944AFB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    - How is this value determined in practice?
+- Isn't 1A too high?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="234">
   <si>
     <t>Specifications</t>
   </si>
@@ -741,6 +760,12 @@
   </si>
   <si>
     <t>14 (13.64)</t>
+  </si>
+  <si>
+    <t>Infineon</t>
+  </si>
+  <si>
+    <t>IPB049N06L3</t>
   </si>
 </sst>
 </file>
@@ -751,7 +776,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -818,8 +843,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -843,6 +874,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -1233,7 +1276,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1263,7 +1306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1329,6 +1371,28 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1337,6 +1401,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1557,6 +1626,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Viktor Neshikj" id="{98535999-FB96-4A15-9443-0B561B4834BD}" userId="S::vnes637@UoA.auckland.ac.nz::c1ccd018-0ab9-471d-aff8-a161acbf54f0" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1820,6 +1895,15 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B31" dT="2024-05-01T12:48:32.66" personId="{98535999-FB96-4A15-9443-0B561B4834BD}" id="{1135DF8B-2E7F-46E9-B040-718C71944AFB}">
+    <text>- How is this value determined in practice?
+- Isn't 1A too high?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -1827,8 +1911,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1863,7 +1947,7 @@
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="57">
         <v>15</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -1874,7 +1958,7 @@
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="58">
         <v>1.3</v>
       </c>
       <c r="C7" s="24" t="s">
@@ -1885,7 +1969,7 @@
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="58">
         <v>9.6999999999999993</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1896,7 +1980,7 @@
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="59">
+      <c r="B9" s="58">
         <v>10</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -1907,7 +1991,7 @@
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="59">
+      <c r="B10" s="58">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -1918,7 +2002,7 @@
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="59">
+      <c r="B11" s="58">
         <v>90</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -1929,7 +2013,7 @@
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="60">
+      <c r="B12" s="59">
         <v>100</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -1969,22 +2053,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B18" s="58">
+      <c r="B18" s="57">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="57">
         <v>4</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F18" s="57">
         <v>10</v>
       </c>
       <c r="G18" s="15" t="s">
@@ -2128,7 +2212,7 @@
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="58">
+      <c r="B29" s="57">
         <f>B6</f>
         <v>15</v>
       </c>
@@ -2140,7 +2224,7 @@
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="59">
+      <c r="B30" s="58">
         <f>F18</f>
         <v>10</v>
       </c>
@@ -2201,7 +2285,7 @@
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="69">
+      <c r="B38" s="68">
         <v>25</v>
       </c>
       <c r="C38" s="23" t="s">
@@ -2239,22 +2323,22 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="58">
+      <c r="B44" s="57">
         <v>2</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="58">
+      <c r="D44" s="57">
         <v>4</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="58">
+      <c r="F44" s="57">
         <v>10</v>
       </c>
       <c r="G44" s="15" t="s">
@@ -2403,8 +2487,8 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2436,10 +2520,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <f>'Operating Conditions'!B38</f>
         <v>25</v>
       </c>
@@ -2448,58 +2532,58 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>3.63</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>2.98</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="52">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="52">
         <v>0.25</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="56">
+      <c r="B11" s="55">
         <v>5</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2522,110 +2606,110 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="60" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="36"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="53">
+      <c r="B19" s="52">
         <v>31</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="36" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="53">
+      <c r="B20" s="52">
         <v>47</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="53">
+      <c r="B21" s="52">
         <v>1460</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="36" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="53">
+      <c r="B22" s="52">
         <v>28.1</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="36" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="53">
+      <c r="B23" s="52">
         <v>40.200000000000003</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="63">
+      <c r="B24" s="62">
         <f>1.8*10^-8</f>
         <v>1.8000000000000002E-8</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="36" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="63">
+      <c r="B25" s="62">
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="56">
+      <c r="B26" s="55">
         <v>0.65</v>
       </c>
-      <c r="C26" s="40"/>
+      <c r="C26" s="39"/>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -2655,24 +2739,24 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="54">
+      <c r="B32" s="53">
         <v>0.15</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="35" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="B33" s="56">
+      <c r="B33" s="55">
         <v>0.43</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="39" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="9"/>
@@ -2699,80 +2783,80 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="69" t="s">
         <v>231</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="71">
+      <c r="B40" s="70">
         <v>0.22</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="36" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="72">
+      <c r="B41" s="71">
         <v>1.4499999999999999E-7</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="36" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="73">
+      <c r="B42" s="72">
         <v>9</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="36" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="72">
+      <c r="B43" s="71">
         <v>1.31E-6</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="36" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="71">
+      <c r="B44" s="70">
         <v>2.27</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="36" t="s">
         <v>87</v>
       </c>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="74">
+      <c r="B45" s="73">
         <v>7.73</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="39" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2807,22 +2891,22 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="67" t="s">
+      <c r="A51" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="64">
+      <c r="B51" s="63">
         <v>2</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="64">
+      <c r="D51" s="63">
         <v>4</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="64">
+      <c r="F51" s="63">
         <v>10</v>
       </c>
       <c r="G51" s="28" t="s">
@@ -2830,104 +2914,140 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="30" t="s">
+      <c r="B52" s="10">
+        <v>2.98</v>
+      </c>
+      <c r="C52" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="29"/>
-      <c r="E52" s="30" t="s">
+      <c r="D52" s="10">
+        <v>2.13</v>
+      </c>
+      <c r="E52" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="29"/>
-      <c r="G52" s="31" t="s">
+      <c r="F52" s="10">
+        <v>1.367</v>
+      </c>
+      <c r="G52" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="30" t="s">
+      <c r="B53" s="10">
+        <v>1.33</v>
+      </c>
+      <c r="C53" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="30" t="s">
+      <c r="D53" s="10">
+        <v>1.27</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="29"/>
-      <c r="G53" s="31" t="s">
+      <c r="F53" s="10">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G53" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="44" t="s">
+      <c r="A54" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="30" t="s">
+      <c r="B54" s="79">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="C54" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="32"/>
-      <c r="E54" s="30" t="s">
+      <c r="D54" s="79">
+        <v>38.479999999999997</v>
+      </c>
+      <c r="E54" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="32"/>
-      <c r="G54" s="31" t="s">
+      <c r="F54" s="79">
+        <v>33.03</v>
+      </c>
+      <c r="G54" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="30" t="s">
+      <c r="B55" s="79">
+        <v>68.67</v>
+      </c>
+      <c r="C55" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="32"/>
-      <c r="E55" s="30" t="s">
+      <c r="D55" s="79">
+        <v>35.08</v>
+      </c>
+      <c r="E55" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="32"/>
-      <c r="G55" s="31" t="s">
+      <c r="F55" s="79">
+        <v>14.51</v>
+      </c>
+      <c r="G55" s="30" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="44" t="s">
+      <c r="A56" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="30" t="s">
+      <c r="B56" s="79">
+        <v>8.99</v>
+      </c>
+      <c r="C56" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="32"/>
-      <c r="E56" s="30" t="s">
+      <c r="D56" s="79">
+        <v>8.01</v>
+      </c>
+      <c r="E56" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="32"/>
-      <c r="G56" s="31" t="s">
+      <c r="F56" s="79">
+        <v>5.47</v>
+      </c>
+      <c r="G56" s="30" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="34" t="s">
+      <c r="B57" s="81">
+        <v>77.66</v>
+      </c>
+      <c r="C57" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="33"/>
-      <c r="E57" s="34" t="s">
+      <c r="D57" s="81">
+        <v>43.09</v>
+      </c>
+      <c r="E57" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="F57" s="33"/>
-      <c r="G57" s="35" t="s">
+      <c r="F57" s="81">
+        <v>19.98</v>
+      </c>
+      <c r="G57" s="34" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2946,8 +3066,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2979,10 +3099,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
@@ -2990,44 +3110,48 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="19">
+        <v>0.38</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="37" t="s">
+      <c r="B8" s="10">
+        <v>1.33</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="52">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="55">
         <v>1</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="39" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3050,20 +3174,24 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" s="74">
+        <v>17.14</v>
+      </c>
       <c r="C16" s="28" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="40" t="s">
+      <c r="B17" s="75">
+        <v>72.930000000000007</v>
+      </c>
+      <c r="C17" s="39" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3086,56 +3214,62 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="36"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="37" t="s">
+      <c r="B25" s="37">
+        <v>35</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="37">
+        <v>330</v>
+      </c>
+      <c r="C26" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="37" t="s">
+      <c r="B27" s="37">
+        <v>52</v>
+      </c>
+      <c r="C27" s="36" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="40" t="s">
+      <c r="B28" s="77"/>
+      <c r="C28" s="78" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3170,59 +3304,71 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="64">
+      <c r="B34" s="63">
         <v>2</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="64">
+      <c r="D34" s="63">
         <v>4</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="64">
+      <c r="F34" s="63">
         <v>10</v>
       </c>
       <c r="G34" s="28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+    <row r="35" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="30" t="s">
+      <c r="B35" s="19">
+        <v>0.38</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30" t="s">
+      <c r="D35" s="19">
+        <v>0.37</v>
+      </c>
+      <c r="E35" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="31" t="s">
+      <c r="F35" s="19">
+        <v>0.31</v>
+      </c>
+      <c r="G35" s="30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+    <row r="36" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="34" t="s">
+      <c r="B36" s="38">
+        <v>7.51</v>
+      </c>
+      <c r="C36" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="34" t="s">
+      <c r="D36" s="38">
+        <v>7.12</v>
+      </c>
+      <c r="E36" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="39"/>
-      <c r="G36" s="35" t="s">
+      <c r="F36" s="38">
+        <v>5</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3235,14 +3381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3274,10 +3420,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -3286,43 +3432,47 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="10">
+        <v>1.98</v>
+      </c>
+      <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="37" t="s">
+      <c r="B8" s="31">
+        <v>3.63</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="52">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="55">
         <v>30</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="39" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3345,88 +3495,108 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="69" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="83" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" s="36"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="37" t="s">
+      <c r="B18" s="84">
+        <v>60</v>
+      </c>
+      <c r="C18" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="84">
+        <v>80</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="37" t="s">
+      <c r="B20" s="84">
+        <v>5</v>
+      </c>
+      <c r="C20" s="36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="37" t="s">
+      <c r="B21" s="84">
+        <v>12</v>
+      </c>
+      <c r="C21" s="36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="37" t="s">
+      <c r="B22" s="84">
+        <v>175</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="37" t="s">
+      <c r="B23" s="84">
+        <v>3.6</v>
+      </c>
+      <c r="C23" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="37" t="s">
+      <c r="B24" s="84">
+        <v>3.9</v>
+      </c>
+      <c r="C24" s="36" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="40" t="s">
+      <c r="B25" s="85">
+        <v>62</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3449,33 +3619,35 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="54">
+      <c r="B30" s="53">
         <v>15</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="53">
+      <c r="B31" s="52">
         <v>1</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="40" t="s">
+      <c r="B32" s="32">
+        <v>15</v>
+      </c>
+      <c r="C32" s="39" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3512,22 +3684,22 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="54">
+      <c r="B38" s="53">
         <v>2</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="64">
+      <c r="D38" s="63">
         <v>4</v>
       </c>
       <c r="E38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="64">
+      <c r="F38" s="63">
         <v>10</v>
       </c>
       <c r="G38" s="28" t="s">
@@ -3535,206 +3707,236 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="30" t="s">
+      <c r="B39">
+        <v>2.96</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30" t="s">
+      <c r="D39" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="E39" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="31" t="s">
+      <c r="F39" s="10">
+        <v>1.325</v>
+      </c>
+      <c r="G39" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="30" t="s">
+      <c r="B40" s="10">
+        <v>1.98</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="30" t="s">
+      <c r="D40" s="10">
+        <v>1.68</v>
+      </c>
+      <c r="E40" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="31" t="s">
+      <c r="F40" s="10">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G40" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="30" t="s">
+      <c r="B41" s="10">
+        <v>1.33</v>
+      </c>
+      <c r="C41" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30" t="s">
+      <c r="D41" s="10">
+        <v>1.27</v>
+      </c>
+      <c r="E41" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="31" t="s">
+      <c r="F41" s="10">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G41" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="30" t="s">
+      <c r="B42" s="31">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C42" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D42" s="32"/>
-      <c r="E42" s="30" t="s">
+      <c r="D42" s="31">
+        <v>1.47</v>
+      </c>
+      <c r="E42" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="31" t="s">
+      <c r="F42" s="31">
+        <v>0.79</v>
+      </c>
+      <c r="G42" s="30" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="B43" s="32"/>
-      <c r="C43" s="30" t="s">
+      <c r="B43" s="31">
+        <v>3.63</v>
+      </c>
+      <c r="C43" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="D43" s="32"/>
-      <c r="E43" s="30" t="s">
+      <c r="D43" s="31">
+        <v>2.74</v>
+      </c>
+      <c r="E43" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="31" t="s">
+      <c r="F43" s="31">
+        <v>1.88</v>
+      </c>
+      <c r="G43" s="30" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="32"/>
-      <c r="C44" s="30" t="s">
+      <c r="B44" s="31"/>
+      <c r="C44" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="32"/>
-      <c r="E44" s="30" t="s">
+      <c r="D44" s="31"/>
+      <c r="E44" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="F44" s="32"/>
-      <c r="G44" s="31" t="s">
+      <c r="F44" s="31"/>
+      <c r="G44" s="30" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="30" t="s">
+      <c r="B45" s="31"/>
+      <c r="C45" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="D45" s="32"/>
-      <c r="E45" s="30" t="s">
+      <c r="D45" s="31"/>
+      <c r="E45" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="F45" s="32"/>
-      <c r="G45" s="31" t="s">
+      <c r="F45" s="31"/>
+      <c r="G45" s="30" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="30" t="s">
+      <c r="B46" s="31"/>
+      <c r="C46" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="30" t="s">
+      <c r="D46" s="31"/>
+      <c r="E46" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="F46" s="32"/>
-      <c r="G46" s="31" t="s">
+      <c r="F46" s="31"/>
+      <c r="G46" s="30" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="30" t="s">
+      <c r="B47" s="31"/>
+      <c r="C47" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="D47" s="32"/>
-      <c r="E47" s="30" t="s">
+      <c r="D47" s="31"/>
+      <c r="E47" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="F47" s="32"/>
-      <c r="G47" s="31" t="s">
+      <c r="F47" s="31"/>
+      <c r="G47" s="30" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
+      <c r="A48" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="30" t="s">
+      <c r="B48" s="31"/>
+      <c r="C48" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="30" t="s">
+      <c r="D48" s="31"/>
+      <c r="E48" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="F48" s="32"/>
-      <c r="G48" s="31" t="s">
+      <c r="F48" s="31"/>
+      <c r="G48" s="30" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="44" t="s">
+      <c r="A49" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="30" t="s">
+      <c r="B49" s="31"/>
+      <c r="C49" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="D49" s="32"/>
-      <c r="E49" s="30" t="s">
+      <c r="D49" s="31"/>
+      <c r="E49" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="31" t="s">
+      <c r="F49" s="31"/>
+      <c r="G49" s="30" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="34" t="s">
+      <c r="B50" s="32"/>
+      <c r="C50" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="D50" s="33"/>
-      <c r="E50" s="34" t="s">
+      <c r="D50" s="32"/>
+      <c r="E50" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="F50" s="33"/>
-      <c r="G50" s="35" t="s">
+      <c r="F50" s="32"/>
+      <c r="G50" s="34" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3757,11 +3959,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="50" t="s">
+      <c r="A56" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="48"/>
-      <c r="C56" s="49" t="s">
+      <c r="B56" s="47"/>
+      <c r="C56" s="48" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3770,6 +3972,7 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3813,10 +4016,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -3825,34 +4028,34 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="37" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="52">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="55">
         <v>30</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="39" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3875,52 +4078,52 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="36"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="35"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="36"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="37" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="37" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="40" t="s">
+      <c r="B20" s="46"/>
+      <c r="C20" s="39" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3955,22 +4158,22 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="66" t="s">
         <v>229</v>
       </c>
-      <c r="B26" s="54">
+      <c r="B26" s="53">
         <v>2</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="64">
+      <c r="D26" s="63">
         <v>4</v>
       </c>
       <c r="E26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="64">
+      <c r="F26" s="63">
         <v>10</v>
       </c>
       <c r="G26" s="28" t="s">
@@ -3978,104 +4181,104 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="30" t="s">
+      <c r="B27" s="31"/>
+      <c r="C27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="30" t="s">
+      <c r="D27" s="31"/>
+      <c r="E27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="31" t="s">
+      <c r="F27" s="31"/>
+      <c r="G27" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="30" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="30" t="s">
+      <c r="D28" s="31"/>
+      <c r="E28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="31" t="s">
+      <c r="F28" s="31"/>
+      <c r="G28" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="30" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="30" t="s">
+      <c r="D29" s="31"/>
+      <c r="E29" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="31" t="s">
+      <c r="F29" s="31"/>
+      <c r="G29" s="30" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="30" t="s">
+      <c r="B30" s="31"/>
+      <c r="C30" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="30" t="s">
+      <c r="D30" s="31"/>
+      <c r="E30" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="31" t="s">
+      <c r="F30" s="31"/>
+      <c r="G30" s="30" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="30" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="30" t="s">
+      <c r="D31" s="31"/>
+      <c r="E31" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="31" t="s">
+      <c r="F31" s="31"/>
+      <c r="G31" s="30" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34" t="s">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34" t="s">
+      <c r="D32" s="32"/>
+      <c r="E32" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="35" t="s">
+      <c r="F32" s="32"/>
+      <c r="G32" s="34" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4098,11 +4301,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49" t="s">
+      <c r="B38" s="47"/>
+      <c r="C38" s="48" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4155,73 +4358,73 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="52">
         <f>'Operating Conditions'!B46</f>
         <v>3.63</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="53">
+      <c r="B8" s="52">
         <f>Capacitor!B26</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="31" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="54">
         <f>Capacitor!B27</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="36" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="53">
+      <c r="B10" s="52">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="56">
+      <c r="B11" s="55">
         <v>5</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4244,31 +4447,31 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="57">
+      <c r="B17" s="56">
         <v>1</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="35" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="37" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="36" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="40" t="s">
+      <c r="B19" s="46"/>
+      <c r="C19" s="39" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4291,31 +4494,31 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="36" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="35" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="53">
+      <c r="B26" s="52">
         <v>100</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="36" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="40" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="39" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4338,107 +4541,107 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="36" t="s">
+      <c r="B33" s="40"/>
+      <c r="C33" s="35" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="37" t="s">
+      <c r="B34" s="31"/>
+      <c r="C34" s="36" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="37" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="68"/>
+      <c r="D35" s="67"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="53">
+      <c r="B36" s="52">
         <v>10</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="36" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="B37" s="53">
+      <c r="B37" s="52">
         <v>1</v>
       </c>
-      <c r="C37" s="37"/>
+      <c r="C37" s="36"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="37" t="s">
+      <c r="B38" s="31"/>
+      <c r="C38" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="D38" s="68"/>
+      <c r="D38" s="67"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="37" t="s">
+      <c r="B39" s="31"/>
+      <c r="C39" s="36" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="B40" s="53">
+      <c r="B40" s="52">
         <v>22</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="36" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="37" t="s">
+      <c r="B41" s="31"/>
+      <c r="C41" s="36" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="37" t="s">
+      <c r="B42" s="31"/>
+      <c r="C42" s="36" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="40" t="s">
+      <c r="B43" s="32"/>
+      <c r="C43" s="39" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(buck-design): :sparkles: Almost completed switch sheet, equation not updated
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C986C4-ED45-4A40-8A8E-744E469E1683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EC1E32-22B4-4C69-9C45-7F6626A1CC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="18645" windowHeight="20985" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -843,12 +843,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -887,7 +881,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1270,13 +1264,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1393,6 +1398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1915,24 +1921,24 @@
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -1943,7 +1949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -2020,16 +2026,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>5</v>
       </c>
@@ -2052,7 +2058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="65" t="s">
         <v>229</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>8</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>40</v>
       </c>
@@ -2144,7 +2150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>9</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>1</v>
       </c>
@@ -2190,14 +2196,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>5</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
@@ -2232,7 +2238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>31</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>29</v>
       </c>
@@ -2254,23 +2260,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
@@ -2292,14 +2298,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>5</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A44" s="65" t="s">
         <v>229</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="16" t="s">
         <v>36</v>
       </c>
@@ -2368,7 +2374,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
         <v>37</v>
       </c>
@@ -2391,7 +2397,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="16" t="s">
         <v>39</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="16" t="s">
         <v>158</v>
       </c>
@@ -2437,7 +2443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
         <v>38</v>
       </c>
@@ -2460,14 +2466,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
     </row>
   </sheetData>
@@ -2487,28 +2493,28 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="77" workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.625" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2519,7 +2525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>49</v>
       </c>
@@ -2531,7 +2537,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>48</v>
       </c>
@@ -2542,7 +2548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>50</v>
       </c>
@@ -2553,7 +2559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
         <v>25</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
         <v>60</v>
       </c>
@@ -2576,7 +2582,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
         <v>62</v>
       </c>
@@ -2587,14 +2593,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
         <v>52</v>
       </c>
@@ -2614,7 +2620,7 @@
       </c>
       <c r="C17" s="28"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>53</v>
       </c>
@@ -2623,7 +2629,7 @@
       </c>
       <c r="C18" s="36"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
         <v>54</v>
       </c>
@@ -2634,7 +2640,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
         <v>58</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
         <v>57</v>
       </c>
@@ -2656,7 +2662,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
         <v>55</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
         <v>56</v>
       </c>
@@ -2678,7 +2684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="43" t="s">
         <v>66</v>
       </c>
@@ -2690,7 +2696,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="43" t="s">
         <v>67</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="44" t="s">
         <v>65</v>
       </c>
@@ -2711,23 +2717,23 @@
       </c>
       <c r="C26" s="39"/>
     </row>
-    <row r="27" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>5</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" s="42" t="s">
         <v>230</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="44" t="s">
         <v>221</v>
       </c>
@@ -2761,17 +2767,17 @@
       </c>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -2782,7 +2788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A39" s="42" t="s">
         <v>73</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
         <v>77</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>81</v>
       </c>
@@ -2815,7 +2821,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>80</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
         <v>83</v>
       </c>
@@ -2837,7 +2843,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
         <v>86</v>
       </c>
@@ -2849,7 +2855,7 @@
       </c>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="44" t="s">
         <v>88</v>
       </c>
@@ -2860,14 +2866,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>5</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A51" s="66" t="s">
         <v>229</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="43" t="s">
         <v>39</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="43" t="s">
         <v>36</v>
       </c>
@@ -2959,7 +2965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="43" t="s">
         <v>92</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="43" t="s">
         <v>93</v>
       </c>
@@ -3005,7 +3011,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="43" t="s">
         <v>94</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="44" t="s">
         <v>95</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3070,24 +3076,24 @@
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>102</v>
       </c>
@@ -3110,7 +3116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>104</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>205</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
         <v>103</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
         <v>106</v>
       </c>
@@ -3155,14 +3161,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
@@ -3173,7 +3179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="s">
         <v>224</v>
       </c>
@@ -3184,7 +3190,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="44" t="s">
         <v>108</v>
       </c>
@@ -3195,14 +3201,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>5</v>
       </c>
@@ -3213,7 +3219,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="42" t="s">
         <v>112</v>
       </c>
@@ -3222,7 +3228,7 @@
       </c>
       <c r="C23" s="35"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="43" t="s">
         <v>111</v>
       </c>
@@ -3231,7 +3237,7 @@
       </c>
       <c r="C24" s="36"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="43" t="s">
         <v>115</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="43" t="s">
         <v>225</v>
       </c>
@@ -3253,7 +3259,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
         <v>117</v>
       </c>
@@ -3264,7 +3270,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="76" t="s">
         <v>119</v>
       </c>
@@ -3273,14 +3279,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>5</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A34" s="66" t="s">
         <v>229</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="43" t="s">
         <v>38</v>
       </c>
@@ -3349,7 +3355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="44" t="s">
         <v>121</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3387,28 +3393,28 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="84" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -3419,7 +3425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>123</v>
       </c>
@@ -3431,7 +3437,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>159</v>
       </c>
@@ -3442,7 +3448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>125</v>
       </c>
@@ -3453,7 +3459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
         <v>124</v>
       </c>
@@ -3465,7 +3471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="44" t="s">
         <v>126</v>
       </c>
@@ -3476,14 +3482,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>5</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="s">
         <v>112</v>
       </c>
@@ -3503,7 +3509,7 @@
       </c>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>129</v>
       </c>
@@ -3512,7 +3518,7 @@
       </c>
       <c r="C17" s="36"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>130</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
         <v>131</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
         <v>132</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
         <v>133</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
         <v>135</v>
       </c>
@@ -3567,7 +3573,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
         <v>138</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="43" t="s">
         <v>137</v>
       </c>
@@ -3589,7 +3595,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="44" t="s">
         <v>165</v>
       </c>
@@ -3600,14 +3606,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>5</v>
       </c>
@@ -3618,7 +3624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A30" s="42" t="s">
         <v>150</v>
       </c>
@@ -3629,7 +3635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
         <v>151</v>
       </c>
@@ -3640,7 +3646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="44" t="s">
         <v>147</v>
       </c>
@@ -3651,16 +3657,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -3683,7 +3689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A38" s="66" t="s">
         <v>229</v>
       </c>
@@ -3706,7 +3712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>140</v>
       </c>
@@ -3729,7 +3735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
         <v>157</v>
       </c>
@@ -3752,7 +3758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>36</v>
       </c>
@@ -3775,7 +3781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>160</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="43" t="s">
         <v>161</v>
       </c>
@@ -3821,133 +3827,175 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="31"/>
+      <c r="B44" s="31">
+        <v>3.45</v>
+      </c>
       <c r="C44" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="31"/>
+      <c r="D44" s="31">
+        <v>3.45</v>
+      </c>
       <c r="E44" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="F44" s="31"/>
+      <c r="F44" s="31">
+        <v>3.45</v>
+      </c>
       <c r="G44" s="30" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="B45" s="31"/>
+      <c r="B45" s="31">
+        <v>10.93</v>
+      </c>
       <c r="C45" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="D45" s="31"/>
+      <c r="D45" s="31">
+        <v>10.93</v>
+      </c>
       <c r="E45" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="F45" s="31"/>
+      <c r="F45" s="31">
+        <v>10.93</v>
+      </c>
       <c r="G45" s="30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="31"/>
+      <c r="B46" s="31">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="C46" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="D46" s="31"/>
+      <c r="D46" s="31">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="E46" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="F46" s="31"/>
+      <c r="F46" s="31">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="G46" s="30" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="31"/>
+      <c r="B47" s="31">
+        <v>22.93</v>
+      </c>
       <c r="C47" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="D47" s="31"/>
+      <c r="D47" s="31">
+        <v>22.93</v>
+      </c>
       <c r="E47" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="F47" s="31"/>
+      <c r="F47" s="31">
+        <v>22.93</v>
+      </c>
       <c r="G47" s="30" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="31"/>
+      <c r="B48" s="86">
+        <v>77</v>
+      </c>
       <c r="C48" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="D48" s="31"/>
+      <c r="D48" s="31">
+        <v>56.44</v>
+      </c>
       <c r="E48" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="F48" s="31"/>
+      <c r="F48" s="31">
+        <v>37.340000000000003</v>
+      </c>
       <c r="G48" s="30" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="31"/>
+      <c r="B49" s="31">
+        <v>15.3</v>
+      </c>
       <c r="C49" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="D49" s="31"/>
+      <c r="D49" s="31">
+        <v>11.01</v>
+      </c>
       <c r="E49" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="F49" s="31"/>
+      <c r="F49" s="31">
+        <v>5.25</v>
+      </c>
       <c r="G49" s="30" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="32"/>
+      <c r="B50" s="32">
+        <v>92.3</v>
+      </c>
       <c r="C50" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="D50" s="32"/>
+      <c r="D50" s="32">
+        <v>67.45</v>
+      </c>
       <c r="E50" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="F50" s="32"/>
+      <c r="F50" s="32">
+        <v>42.59</v>
+      </c>
       <c r="G50" s="34" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
@@ -3958,7 +4006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="49" t="s">
         <v>166</v>
       </c>
@@ -3967,7 +4015,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3987,24 +4035,24 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.125" customWidth="1"/>
-    <col min="2" max="7" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" customWidth="1"/>
+    <col min="2" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -4015,7 +4063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>168</v>
       </c>
@@ -4027,7 +4075,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>169</v>
       </c>
@@ -4036,7 +4084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>124</v>
       </c>
@@ -4048,7 +4096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="44" t="s">
         <v>126</v>
       </c>
@@ -4059,14 +4107,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
@@ -4077,21 +4125,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="35"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="43" t="s">
         <v>129</v>
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="36"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="43" t="s">
         <v>171</v>
       </c>
@@ -4100,7 +4148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>172</v>
       </c>
@@ -4109,7 +4157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
         <v>173</v>
       </c>
@@ -4118,7 +4166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="44" t="s">
         <v>174</v>
       </c>
@@ -4127,14 +4175,14 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
@@ -4157,7 +4205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="66" t="s">
         <v>229</v>
       </c>
@@ -4180,7 +4228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
         <v>140</v>
       </c>
@@ -4197,7 +4245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>9</v>
       </c>
@@ -4214,7 +4262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>175</v>
       </c>
@@ -4231,7 +4279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
         <v>162</v>
       </c>
@@ -4248,7 +4296,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
         <v>177</v>
       </c>
@@ -4265,7 +4313,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="44" t="s">
         <v>95</v>
       </c>
@@ -4282,14 +4330,14 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>5</v>
       </c>
@@ -4300,7 +4348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="49" t="s">
         <v>166</v>
       </c>
@@ -4309,7 +4357,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4328,25 +4376,25 @@
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="3" width="11.875" customWidth="1"/>
-    <col min="4" max="4" width="22.75" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" customWidth="1"/>
+    <col min="2" max="3" width="11.8984375" customWidth="1"/>
+    <col min="4" max="4" width="22.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -4357,7 +4405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>222</v>
       </c>
@@ -4369,7 +4417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="43" t="s">
         <v>206</v>
       </c>
@@ -4381,7 +4429,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
         <v>183</v>
       </c>
@@ -4393,7 +4441,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
         <v>117</v>
       </c>
@@ -4405,7 +4453,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
         <v>124</v>
       </c>
@@ -4417,7 +4465,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
         <v>190</v>
       </c>
@@ -4428,14 +4476,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
@@ -4446,7 +4494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
         <v>185</v>
       </c>
@@ -4457,7 +4505,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>186</v>
       </c>
@@ -4466,7 +4514,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="44" t="s">
         <v>189</v>
       </c>
@@ -4475,14 +4523,14 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>5</v>
       </c>
@@ -4493,7 +4541,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A25" s="42" t="s">
         <v>192</v>
       </c>
@@ -4502,7 +4550,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="50" t="s">
         <v>226</v>
       </c>
@@ -4513,7 +4561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="51" t="s">
         <v>227</v>
       </c>
@@ -4522,14 +4570,14 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>5</v>
       </c>
@@ -4540,7 +4588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="42" t="s">
         <v>209</v>
       </c>
@@ -4549,7 +4597,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="43" t="s">
         <v>208</v>
       </c>
@@ -4558,7 +4606,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="43" t="s">
         <v>199</v>
       </c>
@@ -4568,7 +4616,7 @@
       </c>
       <c r="D35" s="67"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>210</v>
       </c>
@@ -4579,7 +4627,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
         <v>207</v>
       </c>
@@ -4588,7 +4636,7 @@
       </c>
       <c r="C37" s="36"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="43" t="s">
         <v>215</v>
       </c>
@@ -4598,7 +4646,7 @@
       </c>
       <c r="D38" s="67"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="43" t="s">
         <v>217</v>
       </c>
@@ -4607,7 +4655,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="43" t="s">
         <v>211</v>
       </c>
@@ -4618,7 +4666,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="43" t="s">
         <v>212</v>
       </c>
@@ -4627,7 +4675,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="43" t="s">
         <v>213</v>
       </c>
@@ -4636,7 +4684,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="44" t="s">
         <v>223</v>
       </c>
@@ -4645,8 +4693,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>228</v>
       </c>

</xml_diff>

<commit_message>
feat(buck-design): :sparkles: Progress made with buck design
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EC1E32-22B4-4C69-9C45-7F6626A1CC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55114013-9844-42CF-A44C-1618AE2E7FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -63,8 +63,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2B784FD0-A616-45DF-B5B0-7506F5D4E207}</author>
+  </authors>
+  <commentList>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{2B784FD0-A616-45DF-B5B0-7506F5D4E207}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not stated in diode datasheet</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="236">
   <si>
     <t>Specifications</t>
   </si>
@@ -765,7 +783,13 @@
     <t>Infineon</t>
   </si>
   <si>
-    <t>IPB049N06L3</t>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>VS-MBR1045-M3</t>
+  </si>
+  <si>
+    <t>IPP052N06L3</t>
   </si>
 </sst>
 </file>
@@ -776,7 +800,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -843,6 +867,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1281,7 +1311,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1323,9 +1353,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1"/>
@@ -1398,7 +1425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1910,6 +1937,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B20" dT="2024-05-02T03:43:25.90" personId="{98535999-FB96-4A15-9443-0B561B4834BD}" id="{2B784FD0-A616-45DF-B5B0-7506F5D4E207}">
+    <text>Not stated in diode datasheet</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -1917,8 +1952,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A3" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1988,7 @@
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="56">
         <v>15</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -1964,7 +1999,7 @@
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="58">
+      <c r="B7" s="57">
         <v>1.3</v>
       </c>
       <c r="C7" s="24" t="s">
@@ -1975,7 +2010,7 @@
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="57">
         <v>9.6999999999999993</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1986,7 +2021,7 @@
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="58">
+      <c r="B9" s="57">
         <v>10</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -1997,7 +2032,7 @@
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="57">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -2008,7 +2043,7 @@
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="57">
         <v>90</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -2019,7 +2054,7 @@
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="59">
+      <c r="B12" s="58">
         <v>100</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -2059,22 +2094,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="56">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="57">
+      <c r="D18" s="56">
         <v>4</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="57">
+      <c r="F18" s="56">
         <v>10</v>
       </c>
       <c r="G18" s="15" t="s">
@@ -2218,7 +2253,7 @@
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="57">
+      <c r="B29" s="56">
         <f>B6</f>
         <v>15</v>
       </c>
@@ -2230,7 +2265,7 @@
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="58">
+      <c r="B30" s="57">
         <f>F18</f>
         <v>10</v>
       </c>
@@ -2291,7 +2326,7 @@
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="68">
+      <c r="B38" s="67">
         <v>25</v>
       </c>
       <c r="C38" s="23" t="s">
@@ -2329,22 +2364,22 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="65" t="s">
+      <c r="A44" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="57">
+      <c r="B44" s="56">
         <v>2</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="57">
+      <c r="D44" s="56">
         <v>4</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="57">
+      <c r="F44" s="56">
         <v>10</v>
       </c>
       <c r="G44" s="15" t="s">
@@ -2526,10 +2561,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="52">
         <f>'Operating Conditions'!B38</f>
         <v>25</v>
       </c>
@@ -2538,7 +2573,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="31">
@@ -2549,7 +2584,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="31">
@@ -2560,10 +2595,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="51">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -2572,10 +2607,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="51">
         <v>0.25</v>
       </c>
       <c r="C10" s="36" t="s">
@@ -2583,10 +2618,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="54">
         <v>5</v>
       </c>
       <c r="C11" s="39" t="s">
@@ -2612,28 +2647,28 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="60" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="36"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="52">
+      <c r="B19" s="51">
         <v>31</v>
       </c>
       <c r="C19" s="36" t="s">
@@ -2641,10 +2676,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="51">
         <v>47</v>
       </c>
       <c r="C20" s="36" t="s">
@@ -2652,10 +2687,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="52">
+      <c r="B21" s="51">
         <v>1460</v>
       </c>
       <c r="C21" s="36" t="s">
@@ -2663,10 +2698,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="52">
+      <c r="B22" s="51">
         <v>28.1</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -2674,10 +2709,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="52">
+      <c r="B23" s="51">
         <v>40.200000000000003</v>
       </c>
       <c r="C23" s="36" t="s">
@@ -2685,10 +2720,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="62">
+      <c r="B24" s="61">
         <f>1.8*10^-8</f>
         <v>1.8000000000000002E-8</v>
       </c>
@@ -2697,10 +2732,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="62">
+      <c r="B25" s="61">
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
@@ -2709,10 +2744,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26" s="54">
         <v>0.65</v>
       </c>
       <c r="C26" s="39"/>
@@ -2745,10 +2780,10 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="41" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="53">
+      <c r="B32" s="52">
         <v>0.15</v>
       </c>
       <c r="C32" s="35" t="s">
@@ -2756,10 +2791,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="B33" s="55">
+      <c r="B33" s="54">
         <v>0.43</v>
       </c>
       <c r="C33" s="39" t="s">
@@ -2789,10 +2824,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="68" t="s">
         <v>231</v>
       </c>
       <c r="C39" s="35" t="s">
@@ -2800,10 +2835,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="70">
+      <c r="B40" s="69">
         <v>0.22</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -2811,10 +2846,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="71">
+      <c r="B41" s="70">
         <v>1.4499999999999999E-7</v>
       </c>
       <c r="C41" s="36" t="s">
@@ -2822,10 +2857,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="72">
+      <c r="B42" s="71">
         <v>9</v>
       </c>
       <c r="C42" s="36" t="s">
@@ -2833,10 +2868,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="71">
+      <c r="B43" s="70">
         <v>1.31E-6</v>
       </c>
       <c r="C43" s="36" t="s">
@@ -2844,10 +2879,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="70">
+      <c r="B44" s="69">
         <v>2.27</v>
       </c>
       <c r="C44" s="36" t="s">
@@ -2856,10 +2891,10 @@
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="73">
+      <c r="B45" s="72">
         <v>7.73</v>
       </c>
       <c r="C45" s="39" t="s">
@@ -2897,22 +2932,22 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="63">
+      <c r="B51" s="62">
         <v>2</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="63">
+      <c r="D51" s="62">
         <v>4</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="63">
+      <c r="F51" s="62">
         <v>10</v>
       </c>
       <c r="G51" s="28" t="s">
@@ -2920,7 +2955,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="42" t="s">
         <v>39</v>
       </c>
       <c r="B52" s="10">
@@ -2943,7 +2978,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="43" t="s">
+      <c r="A53" s="42" t="s">
         <v>36</v>
       </c>
       <c r="B53" s="10">
@@ -2966,22 +3001,22 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="79">
+      <c r="B54" s="78">
         <v>40.299999999999997</v>
       </c>
-      <c r="C54" s="80" t="s">
+      <c r="C54" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="79">
+      <c r="D54" s="78">
         <v>38.479999999999997</v>
       </c>
-      <c r="E54" s="80" t="s">
+      <c r="E54" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="79">
+      <c r="F54" s="78">
         <v>33.03</v>
       </c>
       <c r="G54" s="30" t="s">
@@ -2989,22 +3024,22 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="43" t="s">
+      <c r="A55" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="79">
+      <c r="B55" s="78">
         <v>68.67</v>
       </c>
-      <c r="C55" s="80" t="s">
+      <c r="C55" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="79">
+      <c r="D55" s="78">
         <v>35.08</v>
       </c>
-      <c r="E55" s="80" t="s">
+      <c r="E55" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="79">
+      <c r="F55" s="78">
         <v>14.51</v>
       </c>
       <c r="G55" s="30" t="s">
@@ -3012,22 +3047,22 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="79">
+      <c r="B56" s="78">
         <v>8.99</v>
       </c>
-      <c r="C56" s="80" t="s">
+      <c r="C56" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="79">
+      <c r="D56" s="78">
         <v>8.01</v>
       </c>
-      <c r="E56" s="80" t="s">
+      <c r="E56" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="79">
+      <c r="F56" s="78">
         <v>5.47</v>
       </c>
       <c r="G56" s="30" t="s">
@@ -3035,22 +3070,22 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="81">
+      <c r="B57" s="80">
         <v>77.66</v>
       </c>
-      <c r="C57" s="82" t="s">
+      <c r="C57" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="81">
+      <c r="D57" s="80">
         <v>43.09</v>
       </c>
-      <c r="E57" s="82" t="s">
+      <c r="E57" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="F57" s="81">
+      <c r="F57" s="80">
         <v>19.98</v>
       </c>
       <c r="G57" s="34" t="s">
@@ -3105,10 +3140,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="52">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
@@ -3117,7 +3152,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>104</v>
       </c>
       <c r="B7" s="19">
@@ -3128,7 +3163,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>205</v>
       </c>
       <c r="B8" s="10">
@@ -3139,10 +3174,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="51">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -3151,10 +3186,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="54">
         <v>1</v>
       </c>
       <c r="C10" s="39" t="s">
@@ -3180,10 +3215,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="74">
+      <c r="B16" s="73">
         <v>17.14</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -3191,10 +3226,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="75">
+      <c r="B17" s="74">
         <v>72.930000000000007</v>
       </c>
       <c r="C17" s="39" t="s">
@@ -3220,25 +3255,25 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="63" t="s">
         <v>113</v>
       </c>
       <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="60" t="s">
         <v>114</v>
       </c>
       <c r="C24" s="36"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>115</v>
       </c>
       <c r="B25" s="37">
@@ -3249,7 +3284,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>225</v>
       </c>
       <c r="B26" s="37">
@@ -3260,7 +3295,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="42" t="s">
         <v>117</v>
       </c>
       <c r="B27" s="37">
@@ -3271,11 +3306,11 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="75" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="77"/>
-      <c r="C28" s="78" t="s">
+      <c r="B28" s="76"/>
+      <c r="C28" s="77" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3310,22 +3345,22 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="62">
         <v>2</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="63">
+      <c r="D34" s="62">
         <v>4</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="63">
+      <c r="F34" s="62">
         <v>10</v>
       </c>
       <c r="G34" s="28" t="s">
@@ -3333,7 +3368,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="42" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="19">
@@ -3356,7 +3391,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="43" t="s">
         <v>121</v>
       </c>
       <c r="B36" s="38">
@@ -3393,8 +3428,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="84" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A17" zoomScale="84" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3426,10 +3461,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="52">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -3438,7 +3473,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>159</v>
       </c>
       <c r="B7" s="10">
@@ -3449,7 +3484,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="31">
@@ -3460,10 +3495,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="51">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -3472,10 +3507,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="54">
         <v>30</v>
       </c>
       <c r="C10" s="39" t="s">
@@ -3501,28 +3536,28 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="69" t="s">
+      <c r="B16" s="68" t="s">
         <v>232</v>
       </c>
       <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="83" t="s">
-        <v>233</v>
+      <c r="B17" s="82" t="s">
+        <v>235</v>
       </c>
       <c r="C17" s="36"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="84">
+      <c r="B18" s="83">
         <v>60</v>
       </c>
       <c r="C18" s="36" t="s">
@@ -3530,10 +3565,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="84">
+      <c r="B19" s="83">
         <v>80</v>
       </c>
       <c r="C19" s="30" t="s">
@@ -3541,10 +3576,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="84">
+      <c r="B20" s="83">
         <v>5</v>
       </c>
       <c r="C20" s="36" t="s">
@@ -3552,10 +3587,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="84">
+      <c r="B21" s="83">
         <v>12</v>
       </c>
       <c r="C21" s="36" t="s">
@@ -3563,10 +3598,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="84">
+      <c r="B22" s="83">
         <v>175</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -3574,10 +3609,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="84">
+      <c r="B23" s="83">
         <v>3.6</v>
       </c>
       <c r="C23" s="36" t="s">
@@ -3585,10 +3620,10 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="84">
+      <c r="B24" s="83">
         <v>3.9</v>
       </c>
       <c r="C24" s="36" t="s">
@@ -3596,10 +3631,10 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="85">
+      <c r="B25" s="84">
         <v>62</v>
       </c>
       <c r="C25" s="39" t="s">
@@ -3625,10 +3660,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="53">
+      <c r="B30" s="52">
         <v>15</v>
       </c>
       <c r="C30" s="35" t="s">
@@ -3636,10 +3671,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="52">
+      <c r="B31" s="51">
         <v>1</v>
       </c>
       <c r="C31" s="36" t="s">
@@ -3647,7 +3682,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="43" t="s">
         <v>147</v>
       </c>
       <c r="B32" s="32">
@@ -3690,22 +3725,22 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="53">
+      <c r="B38" s="52">
         <v>2</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="63">
+      <c r="D38" s="62">
         <v>4</v>
       </c>
       <c r="E38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="63">
+      <c r="F38" s="62">
         <v>10</v>
       </c>
       <c r="G38" s="28" t="s">
@@ -3713,7 +3748,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>140</v>
       </c>
       <c r="B39">
@@ -3736,7 +3771,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="42" t="s">
         <v>157</v>
       </c>
       <c r="B40" s="10">
@@ -3759,7 +3794,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="42" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="10">
@@ -3782,7 +3817,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="42" t="s">
         <v>160</v>
       </c>
       <c r="B42" s="31">
@@ -3805,7 +3840,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="42" t="s">
         <v>161</v>
       </c>
       <c r="B43" s="31">
@@ -3828,7 +3863,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="42" t="s">
         <v>143</v>
       </c>
       <c r="B44" s="31">
@@ -3851,7 +3886,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="42" t="s">
         <v>144</v>
       </c>
       <c r="B45" s="31">
@@ -3874,7 +3909,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="42" t="s">
         <v>152</v>
       </c>
       <c r="B46" s="31">
@@ -3897,7 +3932,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="42" t="s">
         <v>153</v>
       </c>
       <c r="B47" s="31">
@@ -3920,10 +3955,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="86">
+      <c r="B48" s="85">
         <v>77</v>
       </c>
       <c r="C48" s="29" t="s">
@@ -3943,7 +3978,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="42" t="s">
         <v>162</v>
       </c>
       <c r="B49" s="31">
@@ -3966,7 +4001,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="43" t="s">
         <v>95</v>
       </c>
       <c r="B50" s="32">
@@ -4007,11 +4042,13 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="48" t="s">
+      <c r="B56" s="46">
+        <v>35.72</v>
+      </c>
+      <c r="C56" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4025,20 +4062,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.09765625" customWidth="1"/>
-    <col min="2" max="7" width="11.8984375" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -4064,10 +4102,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="52">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -4076,7 +4114,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>169</v>
       </c>
       <c r="B7" s="31"/>
@@ -4085,10 +4123,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="51">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -4097,10 +4135,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="54">
         <v>30</v>
       </c>
       <c r="C9" s="39" t="s">
@@ -4126,52 +4164,62 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="45"/>
+      <c r="B15" s="44" t="s">
+        <v>233</v>
+      </c>
       <c r="C15" s="35"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
       <c r="C16" s="36"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="37">
+        <v>45</v>
+      </c>
       <c r="C17" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="37"/>
+      <c r="B18" s="37">
+        <v>10</v>
+      </c>
       <c r="C18" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="B19" s="37"/>
+      <c r="B19" s="37">
+        <v>0.56999999999999995</v>
+      </c>
       <c r="C19" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="39" t="s">
+      <c r="B20" s="76"/>
+      <c r="C20" s="77" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4206,22 +4254,22 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B26" s="53">
+      <c r="B26" s="52">
         <v>2</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="63">
+      <c r="D26" s="62">
         <v>4</v>
       </c>
       <c r="E26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="62">
         <v>10</v>
       </c>
       <c r="G26" s="28" t="s">
@@ -4229,75 +4277,99 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27">
+        <v>2.96</v>
+      </c>
       <c r="C27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="10">
+        <v>2.1</v>
+      </c>
       <c r="E27" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="31"/>
+      <c r="F27" s="10">
+        <v>1.325</v>
+      </c>
       <c r="G27" s="30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="10">
+        <v>43.88</v>
+      </c>
       <c r="C28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="31"/>
+      <c r="D28" s="10">
+        <v>62.07</v>
+      </c>
       <c r="E28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="31"/>
+      <c r="F28" s="10">
+        <v>71.849999999999994</v>
+      </c>
       <c r="G28" s="30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="31">
+        <v>1.66</v>
+      </c>
       <c r="C29" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="D29" s="31"/>
+      <c r="D29" s="31">
+        <v>0.8</v>
+      </c>
       <c r="E29" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="F29" s="31"/>
+      <c r="F29" s="31">
+        <v>0.37</v>
+      </c>
       <c r="G29" s="30" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="31">
+        <v>0.94</v>
+      </c>
       <c r="C30" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="D30" s="31"/>
+      <c r="D30" s="31">
+        <v>0.46</v>
+      </c>
       <c r="E30" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="31"/>
+      <c r="F30" s="31">
+        <v>0.21</v>
+      </c>
       <c r="G30" s="30" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="42" t="s">
         <v>177</v>
       </c>
       <c r="B31" s="31"/>
@@ -4314,7 +4386,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="43" t="s">
         <v>95</v>
       </c>
       <c r="B32" s="32"/>
@@ -4349,11 +4421,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="48" t="s">
+      <c r="B38" s="46"/>
+      <c r="C38" s="47" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4362,6 +4434,7 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4406,10 +4479,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="52">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
@@ -4418,10 +4491,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="51">
         <f>'Operating Conditions'!B46</f>
         <v>3.63</v>
       </c>
@@ -4430,10 +4503,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="51">
         <f>Capacitor!B26</f>
         <v>330</v>
       </c>
@@ -4442,10 +4515,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="53">
         <f>Capacitor!B27</f>
         <v>52</v>
       </c>
@@ -4454,10 +4527,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="51">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -4466,10 +4539,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="54">
         <v>5</v>
       </c>
       <c r="C11" s="39" t="s">
@@ -4495,10 +4568,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="55">
         <v>1</v>
       </c>
       <c r="C17" s="35" t="s">
@@ -4506,7 +4579,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>186</v>
       </c>
       <c r="B18" s="37"/>
@@ -4515,10 +4588,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="46"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="39" t="s">
         <v>134</v>
       </c>
@@ -4542,7 +4615,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="41" t="s">
         <v>192</v>
       </c>
       <c r="B25" s="40"/>
@@ -4551,10 +4624,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="52">
+      <c r="B26" s="51">
         <v>100</v>
       </c>
       <c r="C26" s="36" t="s">
@@ -4562,7 +4635,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="51" t="s">
+      <c r="A27" s="50" t="s">
         <v>227</v>
       </c>
       <c r="B27" s="32"/>
@@ -4589,7 +4662,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="41" t="s">
         <v>209</v>
       </c>
       <c r="B33" s="40"/>
@@ -4598,7 +4671,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="42" t="s">
         <v>208</v>
       </c>
       <c r="B34" s="31"/>
@@ -4607,20 +4680,20 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="42" t="s">
         <v>199</v>
       </c>
       <c r="B35" s="31"/>
       <c r="C35" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="67"/>
+      <c r="D35" s="66"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="52">
+      <c r="B36" s="51">
         <v>10</v>
       </c>
       <c r="C36" s="36" t="s">
@@ -4628,26 +4701,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="B37" s="52">
+      <c r="B37" s="51">
         <v>1</v>
       </c>
       <c r="C37" s="36"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="42" t="s">
         <v>215</v>
       </c>
       <c r="B38" s="31"/>
       <c r="C38" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="D38" s="67"/>
+      <c r="D38" s="66"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>217</v>
       </c>
       <c r="B39" s="31"/>
@@ -4656,10 +4729,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="B40" s="52">
+      <c r="B40" s="51">
         <v>22</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -4667,7 +4740,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="42" t="s">
         <v>212</v>
       </c>
       <c r="B41" s="31"/>
@@ -4676,7 +4749,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="42" t="s">
         <v>213</v>
       </c>
       <c r="B42" s="31"/>
@@ -4685,7 +4758,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="43" t="s">
         <v>223</v>
       </c>
       <c r="B43" s="32"/>

</xml_diff>

<commit_message>
feat(buck): :sparkles: Almost done with altium
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55114013-9844-42CF-A44C-1618AE2E7FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F98F6-588C-4777-9DD2-1B35AFE9F75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -66,15 +66,24 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={2B784FD0-A616-45DF-B5B0-7506F5D4E207}</author>
+    <author>tc={C4B9823E-A325-4EE1-BAF8-B277917BF74F}</author>
+    <author>tc={DFF7C63C-B98A-4724-ABBD-3FFF1D847E44}</author>
   </authors>
   <commentList>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{2B784FD0-A616-45DF-B5B0-7506F5D4E207}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{C4B9823E-A325-4EE1-BAF8-B277917BF74F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Not stated in diode datasheet</t>
+    How was this value calculated in the design example?</t>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="1" shapeId="0" xr:uid="{DFF7C63C-B98A-4724-ABBD-3FFF1D847E44}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    How was this calculated in design example? Was it chosen arbitrarily under Max Td?</t>
       </text>
     </comment>
   </commentList>
@@ -82,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="238">
   <si>
     <t>Specifications</t>
   </si>
@@ -790,6 +799,12 @@
   </si>
   <si>
     <t>IPP052N06L3</t>
+  </si>
+  <si>
+    <t>18k</t>
+  </si>
+  <si>
+    <t>Assuming same thermal resistance as the other diodes with same case</t>
   </si>
 </sst>
 </file>
@@ -871,7 +886,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -900,18 +915,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFCCCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCFF"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1305,13 +1320,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1359,7 +1383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="2" applyBorder="1"/>
@@ -1409,13 +1432,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1426,6 +1446,23 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1461,9 +1498,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>174625</xdr:colOff>
+      <xdr:colOff>170815</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>135890</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1939,8 +1976,11 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B20" dT="2024-05-02T03:43:25.90" personId="{98535999-FB96-4A15-9443-0B561B4834BD}" id="{2B784FD0-A616-45DF-B5B0-7506F5D4E207}">
-    <text>Not stated in diode datasheet</text>
+  <threadedComment ref="B18" dT="2024-05-02T05:54:47.41" personId="{98535999-FB96-4A15-9443-0B561B4834BD}" id="{C4B9823E-A325-4EE1-BAF8-B277917BF74F}">
+    <text>How was this value calculated in the design example?</text>
+  </threadedComment>
+  <threadedComment ref="B19" dT="2024-05-02T05:55:30.62" personId="{98535999-FB96-4A15-9443-0B561B4834BD}" id="{DFF7C63C-B98A-4724-ABBD-3FFF1D847E44}">
+    <text>How was this calculated in design example? Was it chosen arbitrarily under Max Td?</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1952,8 +1992,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A41" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1988,7 +2028,7 @@
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="55">
         <v>15</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -1999,7 +2039,7 @@
       <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="56">
         <v>1.3</v>
       </c>
       <c r="C7" s="24" t="s">
@@ -2010,7 +2050,7 @@
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="56">
         <v>9.6999999999999993</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -2021,7 +2061,7 @@
       <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="56">
         <v>10</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -2032,7 +2072,7 @@
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="57">
+      <c r="B10" s="56">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -2043,7 +2083,7 @@
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="57">
+      <c r="B11" s="56">
         <v>90</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -2054,7 +2094,7 @@
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="57">
         <v>100</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -2094,22 +2134,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="63" t="s">
         <v>229</v>
       </c>
-      <c r="B18" s="56">
+      <c r="B18" s="55">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="55">
         <v>4</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="56">
+      <c r="F18" s="55">
         <v>10</v>
       </c>
       <c r="G18" s="15" t="s">
@@ -2253,7 +2293,7 @@
       <c r="A29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="56">
+      <c r="B29" s="55">
         <f>B6</f>
         <v>15</v>
       </c>
@@ -2265,7 +2305,7 @@
       <c r="A30" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="57">
+      <c r="B30" s="56">
         <f>F18</f>
         <v>10</v>
       </c>
@@ -2326,7 +2366,7 @@
       <c r="A38" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="67">
+      <c r="B38" s="66">
         <v>25</v>
       </c>
       <c r="C38" s="23" t="s">
@@ -2364,22 +2404,22 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="63" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="56">
+      <c r="B44" s="55">
         <v>2</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D44" s="56">
+      <c r="D44" s="55">
         <v>4</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="56">
+      <c r="F44" s="55">
         <v>10</v>
       </c>
       <c r="G44" s="15" t="s">
@@ -2528,8 +2568,8 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="77" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2564,7 +2604,7 @@
       <c r="A6" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="51">
         <f>'Operating Conditions'!B38</f>
         <v>25</v>
       </c>
@@ -2598,7 +2638,7 @@
       <c r="A9" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="50">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -2610,7 +2650,7 @@
       <c r="A10" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B10" s="50">
         <v>0.25</v>
       </c>
       <c r="C10" s="36" t="s">
@@ -2621,7 +2661,7 @@
       <c r="A11" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="53">
         <v>5</v>
       </c>
       <c r="C11" s="39" t="s">
@@ -2650,7 +2690,7 @@
       <c r="A17" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="28"/>
@@ -2659,7 +2699,7 @@
       <c r="A18" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="59" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="36"/>
@@ -2668,7 +2708,7 @@
       <c r="A19" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="51">
+      <c r="B19" s="50">
         <v>31</v>
       </c>
       <c r="C19" s="36" t="s">
@@ -2679,7 +2719,7 @@
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="51">
+      <c r="B20" s="50">
         <v>47</v>
       </c>
       <c r="C20" s="36" t="s">
@@ -2690,7 +2730,7 @@
       <c r="A21" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="51">
+      <c r="B21" s="50">
         <v>1460</v>
       </c>
       <c r="C21" s="36" t="s">
@@ -2701,7 +2741,7 @@
       <c r="A22" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="51">
+      <c r="B22" s="50">
         <v>28.1</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -2712,7 +2752,7 @@
       <c r="A23" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="51">
+      <c r="B23" s="50">
         <v>40.200000000000003</v>
       </c>
       <c r="C23" s="36" t="s">
@@ -2723,7 +2763,7 @@
       <c r="A24" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="61">
+      <c r="B24" s="60">
         <f>1.8*10^-8</f>
         <v>1.8000000000000002E-8</v>
       </c>
@@ -2735,7 +2775,7 @@
       <c r="A25" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="61">
+      <c r="B25" s="60">
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
@@ -2747,7 +2787,7 @@
       <c r="A26" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="54">
+      <c r="B26" s="53">
         <v>0.65</v>
       </c>
       <c r="C26" s="39"/>
@@ -2783,7 +2823,7 @@
       <c r="A32" s="41" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="52">
+      <c r="B32" s="51">
         <v>0.15</v>
       </c>
       <c r="C32" s="35" t="s">
@@ -2794,7 +2834,7 @@
       <c r="A33" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="B33" s="54">
+      <c r="B33" s="53">
         <v>0.43</v>
       </c>
       <c r="C33" s="39" t="s">
@@ -2827,7 +2867,7 @@
       <c r="A39" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="68" t="s">
+      <c r="B39" s="67" t="s">
         <v>231</v>
       </c>
       <c r="C39" s="35" t="s">
@@ -2838,7 +2878,7 @@
       <c r="A40" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="69">
+      <c r="B40" s="68">
         <v>0.22</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -2849,7 +2889,7 @@
       <c r="A41" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="70">
+      <c r="B41" s="69">
         <v>1.4499999999999999E-7</v>
       </c>
       <c r="C41" s="36" t="s">
@@ -2860,7 +2900,7 @@
       <c r="A42" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="71">
+      <c r="B42" s="70">
         <v>9</v>
       </c>
       <c r="C42" s="36" t="s">
@@ -2871,7 +2911,7 @@
       <c r="A43" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="70">
+      <c r="B43" s="69">
         <v>1.31E-6</v>
       </c>
       <c r="C43" s="36" t="s">
@@ -2882,7 +2922,7 @@
       <c r="A44" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="69">
+      <c r="B44" s="68">
         <v>2.27</v>
       </c>
       <c r="C44" s="36" t="s">
@@ -2894,7 +2934,7 @@
       <c r="A45" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="72">
+      <c r="B45" s="71">
         <v>7.73</v>
       </c>
       <c r="C45" s="39" t="s">
@@ -2932,22 +2972,22 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="62">
+      <c r="B51" s="61">
         <v>2</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D51" s="61">
         <v>4</v>
       </c>
       <c r="E51" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="62">
+      <c r="F51" s="61">
         <v>10</v>
       </c>
       <c r="G51" s="28" t="s">
@@ -3004,19 +3044,19 @@
       <c r="A54" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="78">
+      <c r="B54" s="74">
         <v>40.299999999999997</v>
       </c>
-      <c r="C54" s="79" t="s">
+      <c r="C54" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="78">
+      <c r="D54" s="74">
         <v>38.479999999999997</v>
       </c>
-      <c r="E54" s="79" t="s">
+      <c r="E54" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="F54" s="78">
+      <c r="F54" s="74">
         <v>33.03</v>
       </c>
       <c r="G54" s="30" t="s">
@@ -3027,19 +3067,19 @@
       <c r="A55" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="78">
+      <c r="B55" s="74">
         <v>68.67</v>
       </c>
-      <c r="C55" s="79" t="s">
+      <c r="C55" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="D55" s="78">
+      <c r="D55" s="74">
         <v>35.08</v>
       </c>
-      <c r="E55" s="79" t="s">
+      <c r="E55" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="F55" s="78">
+      <c r="F55" s="74">
         <v>14.51</v>
       </c>
       <c r="G55" s="30" t="s">
@@ -3050,19 +3090,19 @@
       <c r="A56" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="78">
+      <c r="B56" s="74">
         <v>8.99</v>
       </c>
-      <c r="C56" s="79" t="s">
+      <c r="C56" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="78">
+      <c r="D56" s="74">
         <v>8.01</v>
       </c>
-      <c r="E56" s="79" t="s">
+      <c r="E56" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="F56" s="78">
+      <c r="F56" s="74">
         <v>5.47</v>
       </c>
       <c r="G56" s="30" t="s">
@@ -3073,19 +3113,19 @@
       <c r="A57" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="80">
+      <c r="B57" s="76">
         <v>77.66</v>
       </c>
-      <c r="C57" s="81" t="s">
+      <c r="C57" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="80">
+      <c r="D57" s="76">
         <v>43.09</v>
       </c>
-      <c r="E57" s="81" t="s">
+      <c r="E57" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="F57" s="80">
+      <c r="F57" s="76">
         <v>19.98</v>
       </c>
       <c r="G57" s="34" t="s">
@@ -3107,8 +3147,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3143,7 +3183,7 @@
       <c r="A6" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="51">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
@@ -3177,7 +3217,7 @@
       <c r="A9" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="50">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -3189,7 +3229,7 @@
       <c r="A10" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="53">
         <v>1</v>
       </c>
       <c r="C10" s="39" t="s">
@@ -3218,7 +3258,7 @@
       <c r="A16" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="73">
+      <c r="B16" s="72">
         <v>17.14</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -3229,7 +3269,7 @@
       <c r="A17" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="74">
+      <c r="B17" s="73">
         <v>72.930000000000007</v>
       </c>
       <c r="C17" s="39" t="s">
@@ -3258,7 +3298,7 @@
       <c r="A23" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="62" t="s">
         <v>113</v>
       </c>
       <c r="C23" s="35"/>
@@ -3267,7 +3307,7 @@
       <c r="A24" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="59" t="s">
         <v>114</v>
       </c>
       <c r="C24" s="36"/>
@@ -3306,11 +3346,13 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="77" t="s">
+      <c r="B28" s="86">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C28" s="87" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3345,22 +3387,22 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="62">
+      <c r="B34" s="61">
         <v>2</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="61">
         <v>4</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="62">
+      <c r="F34" s="61">
         <v>10</v>
       </c>
       <c r="G34" s="28" t="s">
@@ -3428,8 +3470,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="84" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="84" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3464,7 +3506,7 @@
       <c r="A6" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="51">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -3498,7 +3540,7 @@
       <c r="A9" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="50">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -3510,7 +3552,7 @@
       <c r="A10" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="53">
         <v>30</v>
       </c>
       <c r="C10" s="39" t="s">
@@ -3539,7 +3581,7 @@
       <c r="A16" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="67" t="s">
         <v>232</v>
       </c>
       <c r="C16" s="35"/>
@@ -3548,7 +3590,7 @@
       <c r="A17" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="78" t="s">
         <v>235</v>
       </c>
       <c r="C17" s="36"/>
@@ -3557,7 +3599,7 @@
       <c r="A18" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="83">
+      <c r="B18" s="79">
         <v>60</v>
       </c>
       <c r="C18" s="36" t="s">
@@ -3568,7 +3610,7 @@
       <c r="A19" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="B19" s="83">
+      <c r="B19" s="79">
         <v>80</v>
       </c>
       <c r="C19" s="30" t="s">
@@ -3579,7 +3621,7 @@
       <c r="A20" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="83">
+      <c r="B20" s="79">
         <v>5</v>
       </c>
       <c r="C20" s="36" t="s">
@@ -3590,7 +3632,7 @@
       <c r="A21" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="B21" s="83">
+      <c r="B21" s="79">
         <v>12</v>
       </c>
       <c r="C21" s="36" t="s">
@@ -3601,7 +3643,7 @@
       <c r="A22" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="83">
+      <c r="B22" s="79">
         <v>175</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -3612,7 +3654,7 @@
       <c r="A23" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="83">
+      <c r="B23" s="79">
         <v>3.6</v>
       </c>
       <c r="C23" s="36" t="s">
@@ -3623,7 +3665,7 @@
       <c r="A24" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="83">
+      <c r="B24" s="79">
         <v>3.9</v>
       </c>
       <c r="C24" s="36" t="s">
@@ -3634,7 +3676,7 @@
       <c r="A25" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="84">
+      <c r="B25" s="80">
         <v>62</v>
       </c>
       <c r="C25" s="39" t="s">
@@ -3663,7 +3705,7 @@
       <c r="A30" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="52">
+      <c r="B30" s="51">
         <v>15</v>
       </c>
       <c r="C30" s="35" t="s">
@@ -3674,7 +3716,7 @@
       <c r="A31" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="51">
+      <c r="B31" s="50">
         <v>1</v>
       </c>
       <c r="C31" s="36" t="s">
@@ -3725,22 +3767,22 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="52">
+      <c r="B38" s="51">
         <v>2</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="62">
+      <c r="D38" s="61">
         <v>4</v>
       </c>
       <c r="E38" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="62">
+      <c r="F38" s="61">
         <v>10</v>
       </c>
       <c r="G38" s="28" t="s">
@@ -3958,7 +4000,7 @@
       <c r="A48" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="85">
+      <c r="B48" s="81">
         <v>77</v>
       </c>
       <c r="C48" s="29" t="s">
@@ -4042,13 +4084,13 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="48" t="s">
+      <c r="A56" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="46">
+      <c r="B56" s="45">
         <v>35.72</v>
       </c>
-      <c r="C56" s="47" t="s">
+      <c r="C56" s="46" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4062,14 +4104,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4077,6 +4119,7 @@
     <col min="1" max="1" width="14.09765625" customWidth="1"/>
     <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="11.8984375" customWidth="1"/>
+    <col min="8" max="8" width="11.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
@@ -4105,7 +4148,7 @@
       <c r="A6" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="51">
         <f>'Operating Conditions'!B6</f>
         <v>15</v>
       </c>
@@ -4117,7 +4160,9 @@
       <c r="A7" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="31">
+        <v>1.66</v>
+      </c>
       <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
@@ -4126,7 +4171,7 @@
       <c r="A8" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="50">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -4138,7 +4183,7 @@
       <c r="A9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="53">
         <v>30</v>
       </c>
       <c r="C9" s="39" t="s">
@@ -4181,7 +4226,7 @@
       </c>
       <c r="C16" s="36"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
         <v>171</v>
       </c>
@@ -4192,7 +4237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
         <v>172</v>
       </c>
@@ -4203,7 +4248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="42" t="s">
         <v>173</v>
       </c>
@@ -4214,23 +4259,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="75" t="s">
+    <row r="20" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="77" t="s">
+      <c r="B20" s="86">
+        <v>70</v>
+      </c>
+      <c r="C20" s="87" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="D20" s="83" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:7" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
@@ -4253,30 +4307,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="65" t="s">
+    <row r="26" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="B26" s="52">
+      <c r="B26" s="51">
         <v>2</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="61">
         <v>4</v>
       </c>
       <c r="E26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="62">
+      <c r="F26" s="61">
         <v>10</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="42" t="s">
         <v>140</v>
       </c>
@@ -4299,7 +4353,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="42" t="s">
         <v>9</v>
       </c>
@@ -4322,7 +4376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="42" t="s">
         <v>175</v>
       </c>
@@ -4345,7 +4399,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="42" t="s">
         <v>162</v>
       </c>
@@ -4368,36 +4422,48 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="31"/>
+      <c r="B31" s="31">
+        <v>0</v>
+      </c>
       <c r="C31" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="D31" s="31"/>
+      <c r="D31" s="31">
+        <v>0</v>
+      </c>
       <c r="E31" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="F31" s="31"/>
+      <c r="F31" s="31">
+        <v>0</v>
+      </c>
       <c r="G31" s="30" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="32">
+        <v>0.94</v>
+      </c>
       <c r="C32" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="32">
+        <v>0.94</v>
+      </c>
       <c r="E32" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="32">
+        <v>0.94</v>
+      </c>
       <c r="G32" s="34" t="s">
         <v>180</v>
       </c>
@@ -4421,32 +4487,36 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="46"/>
-      <c r="C38" s="47" t="s">
+      <c r="B38" s="84">
+        <v>95.8</v>
+      </c>
+      <c r="C38" s="85" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D20:H20"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4482,7 +4552,7 @@
       <c r="A6" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="51">
         <f>'Operating Conditions'!B8</f>
         <v>9.6999999999999993</v>
       </c>
@@ -4494,7 +4564,7 @@
       <c r="A7" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="50">
         <f>'Operating Conditions'!B46</f>
         <v>3.63</v>
       </c>
@@ -4506,7 +4576,7 @@
       <c r="A8" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="50">
         <f>Capacitor!B26</f>
         <v>330</v>
       </c>
@@ -4518,7 +4588,7 @@
       <c r="A9" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="53">
+      <c r="B9" s="52">
         <f>Capacitor!B27</f>
         <v>52</v>
       </c>
@@ -4530,7 +4600,7 @@
       <c r="A10" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B10" s="50">
         <f>'Operating Conditions'!B12</f>
         <v>100</v>
       </c>
@@ -4542,7 +4612,7 @@
       <c r="A11" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="53">
         <v>5</v>
       </c>
       <c r="C11" s="39" t="s">
@@ -4571,7 +4641,7 @@
       <c r="A17" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="B17" s="55">
+      <c r="B17" s="54">
         <v>1</v>
       </c>
       <c r="C17" s="35" t="s">
@@ -4579,20 +4649,24 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="92" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="36" t="s">
+      <c r="B18" s="90" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="91" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="88" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="39" t="s">
+      <c r="B19" s="86">
+        <v>320</v>
+      </c>
+      <c r="C19" s="87" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4618,16 +4692,18 @@
       <c r="A25" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="40">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="C25" s="35" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="48" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B26" s="50">
         <v>100</v>
       </c>
       <c r="C26" s="36" t="s">
@@ -4635,10 +4711,12 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="49" t="s">
         <v>227</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="32">
+        <v>159.15</v>
+      </c>
       <c r="C27" s="39" t="s">
         <v>194</v>
       </c>
@@ -4665,7 +4743,9 @@
       <c r="A33" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="B33" s="40"/>
+      <c r="B33" s="40">
+        <v>241.14</v>
+      </c>
       <c r="C33" s="35" t="s">
         <v>197</v>
       </c>
@@ -4674,7 +4754,9 @@
       <c r="A34" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="B34" s="31"/>
+      <c r="B34" s="31">
+        <v>9.27</v>
+      </c>
       <c r="C34" s="36" t="s">
         <v>196</v>
       </c>
@@ -4683,17 +4765,19 @@
       <c r="A35" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B35" s="31"/>
+      <c r="B35" s="31">
+        <v>17.71</v>
+      </c>
       <c r="C35" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="66"/>
+      <c r="D35" s="65"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="B36" s="51">
+      <c r="B36" s="50">
         <v>10</v>
       </c>
       <c r="C36" s="36" t="s">
@@ -4704,7 +4788,7 @@
       <c r="A37" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="B37" s="51">
+      <c r="B37" s="50">
         <v>1</v>
       </c>
       <c r="C37" s="36"/>
@@ -4713,17 +4797,21 @@
       <c r="A38" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="B38" s="31"/>
+      <c r="B38" s="31">
+        <v>32.35</v>
+      </c>
       <c r="C38" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="D38" s="66"/>
+      <c r="D38" s="65"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B39" s="31"/>
+      <c r="B39" s="31">
+        <v>14.63</v>
+      </c>
       <c r="C39" s="36" t="s">
         <v>216</v>
       </c>
@@ -4732,7 +4820,7 @@
       <c r="A40" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="B40" s="51">
+      <c r="B40" s="50">
         <v>22</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -4743,7 +4831,9 @@
       <c r="A41" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="31">
+        <v>0.78</v>
+      </c>
       <c r="C41" s="36" t="s">
         <v>218</v>
       </c>
@@ -4752,7 +4842,9 @@
       <c r="A42" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="31"/>
+      <c r="B42" s="31">
+        <v>4.08</v>
+      </c>
       <c r="C42" s="36" t="s">
         <v>219</v>
       </c>
@@ -4761,7 +4853,9 @@
       <c r="A43" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="32">
+        <v>0.26</v>
+      </c>
       <c r="C43" s="39" t="s">
         <v>220</v>
       </c>
@@ -4777,5 +4871,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(buck + IPT): :sparkles: Completed design
</commit_message>
<xml_diff>
--- a/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
+++ b/Implementation/EE734 Design Report Student Package 2024/EE734 Design Report Student Package 2024/Buck/EE734_Buck_Design_Template_24_UPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnesh\Desktop\ELECTENG - 734\Wirlessly-Powered-RC-Car\Implementation\EE734 Design Report Student Package 2024\EE734 Design Report Student Package 2024\Buck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1F98F6-588C-4777-9DD2-1B35AFE9F75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D31372-A4BC-407B-B540-408FDDEDF876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating Conditions" sheetId="1" r:id="rId1"/>
@@ -815,7 +815,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -882,12 +882,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1335,7 +1329,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1446,23 +1440,19 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1992,8 +1982,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="87" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3147,7 +3137,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -3346,13 +3336,13 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="88" t="s">
+      <c r="A28" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="86">
+      <c r="B28" s="82">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C28" s="87" t="s">
+      <c r="C28" s="39" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3470,7 +3460,7 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScale="84" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -4110,7 +4100,7 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -4260,22 +4250,22 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="86">
+      <c r="B20" s="82">
         <v>70</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="87" t="s">
         <v>237</v>
       </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
     </row>
     <row r="21" spans="1:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
@@ -4487,13 +4477,13 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="89" t="s">
+      <c r="A38" s="84" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="84">
+      <c r="B38" s="45">
         <v>95.8</v>
       </c>
-      <c r="C38" s="85" t="s">
+      <c r="C38" s="46" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4515,8 +4505,8 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4649,24 +4639,24 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="91" t="s">
+      <c r="C18" s="36" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="83" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="86">
+      <c r="B19" s="82">
         <v>320</v>
       </c>
-      <c r="C19" s="87" t="s">
+      <c r="C19" s="39" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>